<commit_message>
Added some new cards, also added Game Design Doc
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -10,11 +10,12 @@
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
   <si>
     <t>Card ID</t>
   </si>
@@ -260,9 +261,6 @@
     <t>Dying Nobleman</t>
   </si>
   <si>
-    <t>The Plaguedoctor</t>
-  </si>
-  <si>
     <t>Burly Zombie</t>
   </si>
   <si>
@@ -293,6 +291,9 @@
     <t>Black Market</t>
   </si>
   <si>
+    <t>Discard a card in your hand and gain gold equal to its cost.</t>
+  </si>
+  <si>
     <t>Done?</t>
   </si>
   <si>
@@ -302,7 +303,31 @@
     <t>N</t>
   </si>
   <si>
-    <t>Discard a card in your hand or kill a creature on your side of the field, and gain gold equal to its cost.</t>
+    <t>Mad Scientist</t>
+  </si>
+  <si>
+    <t>Pustulent Zombie</t>
+  </si>
+  <si>
+    <t>When this minion is killed, you can bury it instead. If this minion battles an opponents minion, give it 1 poison counter.</t>
+  </si>
+  <si>
+    <t>Combat Medic</t>
+  </si>
+  <si>
+    <t>When this minion is summoned, you can restore 2 health to a minion on the field. You can pay 2 gold, restore 2 health to a minion on the field.</t>
+  </si>
+  <si>
+    <t>Immunity</t>
+  </si>
+  <si>
+    <t>Remove all poison counters from all minions on your side of the field.</t>
+  </si>
+  <si>
+    <t>Antidote</t>
+  </si>
+  <si>
+    <t>Remove all poison counters from a minion on your side of the field.</t>
   </si>
 </sst>
 </file>
@@ -375,28 +400,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -711,7 +715,7 @@
   <dimension ref="D2:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -979,7 +983,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K11" t="s">
         <v>51</v>
@@ -1005,7 +1009,7 @@
         <v>2</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K12" t="s">
         <v>51</v>
@@ -1109,7 +1113,7 @@
         <v>30</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K16" t="s">
         <v>51</v>
@@ -1161,7 +1165,7 @@
         <v>1</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K18" t="s">
         <v>51</v>
@@ -1171,8 +1175,8 @@
       <c r="D19" s="7">
         <v>17</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>38</v>
+      <c r="E19" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>12</v>
@@ -1187,7 +1191,7 @@
         <v>3</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K19" t="s">
         <v>51</v>
@@ -1198,7 +1202,7 @@
         <v>18</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>12</v>
@@ -1213,7 +1217,7 @@
         <v>5</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K20" t="s">
         <v>51</v>
@@ -1224,7 +1228,7 @@
         <v>19</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>12</v>
@@ -1239,7 +1243,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K21" t="s">
         <v>51</v>
@@ -1250,7 +1254,7 @@
         <v>20</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>11</v>
@@ -1258,8 +1262,14 @@
       <c r="G22" s="4">
         <v>0</v>
       </c>
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
+      <c r="I22" s="4">
+        <v>0</v>
+      </c>
       <c r="J22" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="K22" t="s">
         <v>51</v>
@@ -1269,21 +1279,93 @@
       <c r="D23" s="7">
         <v>21</v>
       </c>
+      <c r="E23" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="4">
+        <v>6</v>
+      </c>
+      <c r="H23" s="4">
+        <v>10</v>
+      </c>
+      <c r="I23" s="4">
+        <v>1</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="24" spans="4:11">
       <c r="D24" s="7">
         <v>22</v>
       </c>
+      <c r="E24" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="4">
+        <v>2</v>
+      </c>
+      <c r="H24" s="4">
+        <v>2</v>
+      </c>
+      <c r="I24" s="4">
+        <v>2</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="25" spans="4:11">
       <c r="D25" s="7">
         <v>23</v>
       </c>
+      <c r="E25" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="4">
+        <v>5</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="26" spans="4:11">
       <c r="D26" s="7">
         <v>24</v>
       </c>
+      <c r="E26" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="4">
+        <v>2</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0</v>
+      </c>
+      <c r="I26" s="4">
+        <v>0</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="27" spans="4:11">
       <c r="D27" s="7">
@@ -1667,13 +1749,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:J102 K2">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$F2="LORD"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$F2="MINION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$F2="UTILITY"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added Bloated Body and Betrayal to the card list
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\ce301_thorn_t\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075"/>
   </bookViews>
@@ -10,12 +15,11 @@
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
   <si>
     <t>Card ID</t>
   </si>
@@ -264,9 +268,6 @@
     <t>Burly Zombie</t>
   </si>
   <si>
-    <t>Dissappearing frog</t>
-  </si>
-  <si>
     <t>When this minion is called upon, kill all minions on your opponents field, and discard all cards in their hand. This card cannot be summoned by card abilities, except "Occult Devotee".</t>
   </si>
   <si>
@@ -282,9 +283,6 @@
     <t>When this minion is summoned, you can pay 2 gold, ressurect a creature from your discard pile to the battlefield, but put it to 1 health.</t>
   </si>
   <si>
-    <t>When this minion is killed, you can bury it instead. When this minion is ressurected, it comes back with 7 strength, and 7 health.</t>
-  </si>
-  <si>
     <t>When this minion reaches 0 health from combat, you can return it to your hand from the battlefield instead of killing it.</t>
   </si>
   <si>
@@ -328,13 +326,43 @@
   </si>
   <si>
     <t>Remove all poison counters from a minion on your side of the field.</t>
+  </si>
+  <si>
+    <t>Negotiator</t>
+  </si>
+  <si>
+    <t>While this unit is on the field - you do not pay wages for your units.</t>
+  </si>
+  <si>
+    <t>Toxic Frog</t>
+  </si>
+  <si>
+    <t>You can return this card to your hand, place 3 poison counters on an enemy unit.</t>
+  </si>
+  <si>
+    <t>Betrayal</t>
+  </si>
+  <si>
+    <t>Kill a Unit you control, then summon a Unit from your deck with the same cost.</t>
+  </si>
+  <si>
+    <t>When this minion is killed, you can bury it instead. When this minion is ressurected, its strength and health becomes 7.</t>
+  </si>
+  <si>
+    <t>Illusionary frog</t>
+  </si>
+  <si>
+    <t>Bloated Body</t>
+  </si>
+  <si>
+    <t>When this unit is killed, deal 3 damage to all other units on the battlefield.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,6 +452,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -470,7 +506,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -502,9 +538,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -536,6 +573,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -711,14 +749,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="9.140625" style="7"/>
     <col min="5" max="5" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
@@ -729,7 +767,7 @@
     <col min="10" max="10" width="163.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:11">
+    <row r="2" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -752,10 +790,10 @@
         <v>3</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="4:11">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D3" s="6">
         <v>1</v>
       </c>
@@ -778,10 +816,10 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="4:11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D4" s="6">
         <v>2</v>
       </c>
@@ -804,10 +842,10 @@
         <v>20</v>
       </c>
       <c r="K4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="4:11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D5" s="6">
         <v>3</v>
       </c>
@@ -830,10 +868,10 @@
         <v>19</v>
       </c>
       <c r="K5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="4:11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D6" s="6">
         <v>4</v>
       </c>
@@ -856,10 +894,10 @@
         <v>18</v>
       </c>
       <c r="K6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="4:11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D7" s="6">
         <v>5</v>
       </c>
@@ -882,10 +920,10 @@
         <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="4:11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D8" s="6">
         <v>6</v>
       </c>
@@ -908,10 +946,10 @@
         <v>26</v>
       </c>
       <c r="K8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="4:11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D9" s="6">
         <v>7</v>
       </c>
@@ -934,10 +972,10 @@
         <v>22</v>
       </c>
       <c r="K9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="4:11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D10" s="6">
         <v>8</v>
       </c>
@@ -960,10 +998,10 @@
         <v>27</v>
       </c>
       <c r="K10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="4:11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D11" s="7">
         <v>9</v>
       </c>
@@ -983,13 +1021,13 @@
         <v>1</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="4:11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D12" s="7">
         <v>10</v>
       </c>
@@ -1009,13 +1047,13 @@
         <v>2</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="4:11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D13" s="7">
         <v>11</v>
       </c>
@@ -1038,10 +1076,10 @@
         <v>29</v>
       </c>
       <c r="K13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="4:11">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D14" s="7">
         <v>12</v>
       </c>
@@ -1064,10 +1102,10 @@
         <v>31</v>
       </c>
       <c r="K14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="4:11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D15" s="7">
         <v>13</v>
       </c>
@@ -1090,10 +1128,10 @@
         <v>34</v>
       </c>
       <c r="K15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="4:11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D16" s="7">
         <v>14</v>
       </c>
@@ -1113,13 +1151,13 @@
         <v>30</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="4:11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D17" s="7">
         <v>15</v>
       </c>
@@ -1142,10 +1180,10 @@
         <v>36</v>
       </c>
       <c r="K17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="4:11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D18" s="7">
         <v>16</v>
       </c>
@@ -1165,18 +1203,18 @@
         <v>1</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="4:11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D19" s="7">
         <v>17</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>12</v>
@@ -1191,13 +1229,13 @@
         <v>3</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="4:11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D20" s="7">
         <v>18</v>
       </c>
@@ -1217,18 +1255,18 @@
         <v>5</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="K20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="4:11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D21" s="7">
         <v>19</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>12</v>
@@ -1243,18 +1281,18 @@
         <v>2</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="4:11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D22" s="7">
         <v>20</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>11</v>
@@ -1269,18 +1307,18 @@
         <v>0</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="4:11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D23" s="7">
         <v>21</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>12</v>
@@ -1295,15 +1333,15 @@
         <v>1</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="4:11">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D24" s="7">
         <v>22</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>12</v>
@@ -1318,15 +1356,15 @@
         <v>2</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="4:11">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D25" s="7">
         <v>23</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>11</v>
@@ -1341,15 +1379,15 @@
         <v>0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="4:11">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D26" s="7">
         <v>24</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>11</v>
@@ -1364,385 +1402,457 @@
         <v>0</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="4:11">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D27" s="7">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="4:11">
+      <c r="E27" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="4">
+        <v>5</v>
+      </c>
+      <c r="H27" s="4">
+        <v>1</v>
+      </c>
+      <c r="I27" s="4">
+        <v>1</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D28" s="7">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="4:11">
+      <c r="E28" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="4">
+        <v>3</v>
+      </c>
+      <c r="H28" s="4">
+        <v>2</v>
+      </c>
+      <c r="I28" s="4">
+        <v>2</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D29" s="7">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="4:11">
+      <c r="E29" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="4">
+        <v>2</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0</v>
+      </c>
+      <c r="I29" s="4">
+        <v>0</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D30" s="7">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="4:11">
+      <c r="E30" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="4">
+        <v>4</v>
+      </c>
+      <c r="H30" s="4">
+        <v>1</v>
+      </c>
+      <c r="I30" s="4">
+        <v>1</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D31" s="7">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="4:11">
+    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D32" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="4:4">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="7">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="4:4">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="7">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="4:4">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="7">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="4:4">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="7">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="4:4">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="7">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="4:4">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="7">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="4:4">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="7">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="4:4">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="7">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="4:4">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="7">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="4:4">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="7">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="4:4">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="7">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="4:4">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="7">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="4:4">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" s="7">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="4:4">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="7">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="4:4">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" s="7">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="4:4">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="7">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="4:4">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="7">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="4:4">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="7">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="4:4">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="7">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="4:4">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="7">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="4:4">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="7">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="4:4">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="7">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="4:4">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" s="7">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="4:4">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" s="7">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="4:4">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" s="7">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="4:4">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D58" s="7">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="4:4">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D59" s="7">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="4:4">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D60" s="7">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="4:4">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D61" s="7">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="4:4">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D62" s="7">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="4:4">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D63" s="7">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="4:4">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D64" s="7">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="4:4">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" s="7">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="4:4">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="7">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="4:4">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" s="7">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="4:4">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" s="7">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="4:4">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D69" s="7">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="4:4">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D70" s="7">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="4:4">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D71" s="7">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="4:4">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D72" s="7">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="4:4">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D73" s="7">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="4:4">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D74" s="7">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="4:4">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D75" s="7">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="4:4">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D76" s="7">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="4:4">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D77" s="7">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="4:4">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D78" s="7">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="4:4">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D79" s="7">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="4:4">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D80" s="7">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="4:4">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D81" s="7">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="4:4">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D82" s="7">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="4:4">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D83" s="7">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="4:4">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D84" s="7">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="4:4">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D85" s="7">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="4:4">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D86" s="7">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="4:4">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D87" s="7">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="4:4">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D88" s="7">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="4:4">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D89" s="7">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="4:4">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D90" s="7">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="4:4">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D91" s="7">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="4:4">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D92" s="7">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="4:4">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D93" s="7">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="4:4">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D94" s="7">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="4:4">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D95" s="7">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="4:4">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D96" s="7">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="4:4">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D97" s="7">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="4:4">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D98" s="7">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="4:4">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D99" s="7">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="4:4">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D100" s="7">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="4:4">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D101" s="7">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="4:4">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D102" s="7">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Added game-specific terminology to the cards list
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -232,9 +232,6 @@
     <t>If this card defeats an opponents minion in battle, you can pay 1 coin bury it to your side of the battlefield.</t>
   </si>
   <si>
-    <t>You can return this card to your hand, then deal 2 damage to each of your opponents minions.</t>
-  </si>
-  <si>
     <t>Withdrawal</t>
   </si>
   <si>
@@ -271,21 +268,12 @@
     <t>When this minion is called upon, kill all minions on your opponents field, and discard all cards in their hand. This card cannot be summoned by card abilities, except "Occult Devotee".</t>
   </si>
   <si>
-    <t>You can pay 3 coins, return this minion to your hand, then you can take control of 1 minion your opponent controls.</t>
-  </si>
-  <si>
-    <t>You can pay 3 coins, return this minion to your hand, then you can add 1 "Frog" card to your hand, from your deck.</t>
-  </si>
-  <si>
     <t>When this minion is killed, gain 6 gold.</t>
   </si>
   <si>
     <t>When this minion is summoned, you can pay 2 gold, ressurect a creature from your discard pile to the battlefield, but put it to 1 health.</t>
   </si>
   <si>
-    <t>When this minion reaches 0 health from combat, you can return it to your hand from the battlefield instead of killing it.</t>
-  </si>
-  <si>
     <t>Black Market</t>
   </si>
   <si>
@@ -337,9 +325,6 @@
     <t>Toxic Frog</t>
   </si>
   <si>
-    <t>You can return this card to your hand, place 3 poison counters on an enemy unit.</t>
-  </si>
-  <si>
     <t>Betrayal</t>
   </si>
   <si>
@@ -356,6 +341,126 @@
   </si>
   <si>
     <t>When this unit is killed, deal 3 damage to all other units on the battlefield.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">You can </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">bounce </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>this unit, then deal 2 damage to each of your opponents minions.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">You can pay 3 coins, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">bounce </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>this unit, then you can take control of 1 minion your opponent controls.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">You can pay 3 coins, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bounce</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> this unit, then you can add 1 "Frog" card to your hand, from your deck.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When this minion reaches 0 health from combat, you can </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">bounce </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>this unit instead of killing it.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">You can </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">bounce </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>this unit, place 3 poison counters on an enemy unit.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -753,7 +858,7 @@
   <dimension ref="D2:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,7 +895,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="4:11" x14ac:dyDescent="0.25">
@@ -816,7 +921,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="4:11" x14ac:dyDescent="0.25">
@@ -842,7 +947,7 @@
         <v>20</v>
       </c>
       <c r="K4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="4:11" x14ac:dyDescent="0.25">
@@ -868,7 +973,7 @@
         <v>19</v>
       </c>
       <c r="K5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="4:11" x14ac:dyDescent="0.25">
@@ -894,7 +999,7 @@
         <v>18</v>
       </c>
       <c r="K6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="4:11" x14ac:dyDescent="0.25">
@@ -920,7 +1025,7 @@
         <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="4:11" x14ac:dyDescent="0.25">
@@ -946,7 +1051,7 @@
         <v>26</v>
       </c>
       <c r="K8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="4:11" x14ac:dyDescent="0.25">
@@ -972,7 +1077,7 @@
         <v>22</v>
       </c>
       <c r="K9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="4:11" x14ac:dyDescent="0.25">
@@ -995,10 +1100,10 @@
         <v>5</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="K10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="4:11" x14ac:dyDescent="0.25">
@@ -1021,10 +1126,10 @@
         <v>1</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="K11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="4:11" x14ac:dyDescent="0.25">
@@ -1047,10 +1152,10 @@
         <v>2</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="K12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="4:11" x14ac:dyDescent="0.25">
@@ -1058,7 +1163,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>11</v>
@@ -1073,10 +1178,10 @@
         <v>0</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="4:11" x14ac:dyDescent="0.25">
@@ -1084,7 +1189,7 @@
         <v>12</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>11</v>
@@ -1099,10 +1204,10 @@
         <v>0</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="4:11" x14ac:dyDescent="0.25">
@@ -1110,7 +1215,7 @@
         <v>13</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>12</v>
@@ -1125,10 +1230,10 @@
         <v>2</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="4:11" x14ac:dyDescent="0.25">
@@ -1136,7 +1241,7 @@
         <v>14</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>12</v>
@@ -1151,10 +1256,10 @@
         <v>30</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
@@ -1162,7 +1267,7 @@
         <v>15</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>11</v>
@@ -1177,10 +1282,10 @@
         <v>0</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K17" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.25">
@@ -1188,7 +1293,7 @@
         <v>16</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>12</v>
@@ -1203,10 +1308,10 @@
         <v>1</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.25">
@@ -1214,7 +1319,7 @@
         <v>17</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>12</v>
@@ -1229,10 +1334,10 @@
         <v>3</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="K19" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.25">
@@ -1240,7 +1345,7 @@
         <v>18</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>12</v>
@@ -1255,10 +1360,10 @@
         <v>5</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="K20" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.25">
@@ -1266,7 +1371,7 @@
         <v>19</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>12</v>
@@ -1281,10 +1386,10 @@
         <v>2</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="K21" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.25">
@@ -1292,7 +1397,7 @@
         <v>20</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>11</v>
@@ -1307,10 +1412,10 @@
         <v>0</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K22" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="4:11" x14ac:dyDescent="0.25">
@@ -1318,7 +1423,7 @@
         <v>21</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>12</v>
@@ -1333,7 +1438,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="4:11" x14ac:dyDescent="0.25">
@@ -1341,7 +1446,7 @@
         <v>22</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>12</v>
@@ -1356,7 +1461,7 @@
         <v>2</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="4:11" x14ac:dyDescent="0.25">
@@ -1364,7 +1469,7 @@
         <v>23</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>11</v>
@@ -1379,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="4:11" x14ac:dyDescent="0.25">
@@ -1387,7 +1492,7 @@
         <v>24</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>11</v>
@@ -1402,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="4:11" x14ac:dyDescent="0.25">
@@ -1410,7 +1515,7 @@
         <v>25</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>12</v>
@@ -1425,7 +1530,7 @@
         <v>1</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="4:11" x14ac:dyDescent="0.25">
@@ -1433,7 +1538,7 @@
         <v>26</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>12</v>
@@ -1448,7 +1553,7 @@
         <v>2</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="4:11" x14ac:dyDescent="0.25">
@@ -1456,7 +1561,7 @@
         <v>27</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>11</v>
@@ -1471,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="4:11" x14ac:dyDescent="0.25">
@@ -1479,7 +1584,7 @@
         <v>28</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>12</v>
@@ -1494,7 +1599,7 @@
         <v>1</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="4:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed the wording of Concrete Floor to use different terminology
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -217,9 +217,6 @@
     </r>
   </si>
   <si>
-    <t>Destroy a buried minion.</t>
-  </si>
-  <si>
     <t>Seismic Frog</t>
   </si>
   <si>
@@ -461,6 +458,9 @@
       </rPr>
       <t>this unit, place 3 poison counters on an enemy unit.</t>
     </r>
+  </si>
+  <si>
+    <t>Send a buried minion to it's owner's Discard Pile.</t>
   </si>
 </sst>
 </file>
@@ -858,7 +858,7 @@
   <dimension ref="D2:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,7 +895,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="4:11" x14ac:dyDescent="0.25">
@@ -921,7 +921,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="4:11" x14ac:dyDescent="0.25">
@@ -947,7 +947,7 @@
         <v>20</v>
       </c>
       <c r="K4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="4:11" x14ac:dyDescent="0.25">
@@ -973,7 +973,7 @@
         <v>19</v>
       </c>
       <c r="K5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="4:11" x14ac:dyDescent="0.25">
@@ -999,7 +999,7 @@
         <v>18</v>
       </c>
       <c r="K6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="4:11" x14ac:dyDescent="0.25">
@@ -1025,7 +1025,7 @@
         <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="4:11" x14ac:dyDescent="0.25">
@@ -1048,10 +1048,10 @@
         <v>2</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="4:11" x14ac:dyDescent="0.25">
@@ -1074,10 +1074,10 @@
         <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="K9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="4:11" x14ac:dyDescent="0.25">
@@ -1085,7 +1085,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>12</v>
@@ -1100,10 +1100,10 @@
         <v>5</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="4:11" x14ac:dyDescent="0.25">
@@ -1111,7 +1111,7 @@
         <v>9</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>12</v>
@@ -1126,10 +1126,10 @@
         <v>1</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="4:11" x14ac:dyDescent="0.25">
@@ -1137,7 +1137,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>12</v>
@@ -1152,10 +1152,10 @@
         <v>2</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="4:11" x14ac:dyDescent="0.25">
@@ -1163,7 +1163,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>11</v>
@@ -1178,10 +1178,10 @@
         <v>0</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="4:11" x14ac:dyDescent="0.25">
@@ -1189,7 +1189,7 @@
         <v>12</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>11</v>
@@ -1204,10 +1204,10 @@
         <v>0</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="4:11" x14ac:dyDescent="0.25">
@@ -1215,7 +1215,7 @@
         <v>13</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>12</v>
@@ -1230,10 +1230,10 @@
         <v>2</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="4:11" x14ac:dyDescent="0.25">
@@ -1241,7 +1241,7 @@
         <v>14</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>12</v>
@@ -1256,10 +1256,10 @@
         <v>30</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
@@ -1267,7 +1267,7 @@
         <v>15</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>11</v>
@@ -1282,10 +1282,10 @@
         <v>0</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.25">
@@ -1293,7 +1293,7 @@
         <v>16</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>12</v>
@@ -1308,10 +1308,10 @@
         <v>1</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.25">
@@ -1319,7 +1319,7 @@
         <v>17</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>12</v>
@@ -1334,10 +1334,10 @@
         <v>3</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.25">
@@ -1345,7 +1345,7 @@
         <v>18</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>12</v>
@@ -1360,10 +1360,10 @@
         <v>5</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.25">
@@ -1371,7 +1371,7 @@
         <v>19</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>12</v>
@@ -1386,10 +1386,10 @@
         <v>2</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.25">
@@ -1397,7 +1397,7 @@
         <v>20</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>11</v>
@@ -1412,10 +1412,10 @@
         <v>0</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="4:11" x14ac:dyDescent="0.25">
@@ -1423,7 +1423,7 @@
         <v>21</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>12</v>
@@ -1438,7 +1438,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="4:11" x14ac:dyDescent="0.25">
@@ -1446,7 +1446,7 @@
         <v>22</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>12</v>
@@ -1461,7 +1461,7 @@
         <v>2</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="4:11" x14ac:dyDescent="0.25">
@@ -1469,7 +1469,7 @@
         <v>23</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>11</v>
@@ -1484,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="4:11" x14ac:dyDescent="0.25">
@@ -1492,7 +1492,7 @@
         <v>24</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>11</v>
@@ -1507,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="4:11" x14ac:dyDescent="0.25">
@@ -1515,7 +1515,7 @@
         <v>25</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>12</v>
@@ -1524,13 +1524,13 @@
         <v>5</v>
       </c>
       <c r="H27" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I27" s="4">
         <v>1</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="4:11" x14ac:dyDescent="0.25">
@@ -1538,7 +1538,7 @@
         <v>26</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>12</v>
@@ -1553,7 +1553,7 @@
         <v>2</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="4:11" x14ac:dyDescent="0.25">
@@ -1561,7 +1561,7 @@
         <v>27</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>11</v>
@@ -1576,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="4:11" x14ac:dyDescent="0.25">
@@ -1584,7 +1584,7 @@
         <v>28</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>12</v>
@@ -1599,7 +1599,7 @@
         <v>1</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="4:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added 4 new cards to the card list
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="77">
   <si>
     <t>Card ID</t>
   </si>
@@ -461,6 +461,30 @@
   </si>
   <si>
     <t>Send a buried minion to it's owner's Discard Pile.</t>
+  </si>
+  <si>
+    <t>Sleight of Hand</t>
+  </si>
+  <si>
+    <t>Shuffle one card back into your deck, then draw 2 cards.</t>
+  </si>
+  <si>
+    <t>Infiltrator</t>
+  </si>
+  <si>
+    <t>When you hire this card, kill one Unit on your opponent's side of the field, then switch control of this card.</t>
+  </si>
+  <si>
+    <t>Artillery</t>
+  </si>
+  <si>
+    <t>Treachary</t>
+  </si>
+  <si>
+    <t>Deal 2 damage to all Minions your opponent controls.</t>
+  </si>
+  <si>
+    <t>Hire one Unit from your opponent's side of the field.</t>
   </si>
 </sst>
 </file>
@@ -858,7 +882,7 @@
   <dimension ref="D2:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1567,7 +1591,7 @@
         <v>11</v>
       </c>
       <c r="G29" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H29" s="4">
         <v>0</v>
@@ -1606,88 +1630,160 @@
       <c r="D31" s="7">
         <v>29</v>
       </c>
+      <c r="E31" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="4">
+        <v>4</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0</v>
+      </c>
+      <c r="I31" s="4">
+        <v>0</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="32" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D32" s="7">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="4">
+        <v>4</v>
+      </c>
+      <c r="H32" s="4">
+        <v>1</v>
+      </c>
+      <c r="I32" s="4">
+        <v>1</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D33" s="7">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="4">
+        <v>5</v>
+      </c>
+      <c r="H33" s="4">
+        <v>0</v>
+      </c>
+      <c r="I33" s="4">
+        <v>0</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D34" s="7">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="4">
+        <v>8</v>
+      </c>
+      <c r="H34" s="4">
+        <v>0</v>
+      </c>
+      <c r="I34" s="4">
+        <v>0</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D35" s="7">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D36" s="7">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D37" s="7">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D38" s="7">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D39" s="7">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D40" s="7">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D41" s="7">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D42" s="7">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D43" s="7">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D44" s="7">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D45" s="7">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D46" s="7">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D47" s="7">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D48" s="7">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Fixed wording on Sleight of Hand
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -466,9 +466,6 @@
     <t>Sleight of Hand</t>
   </si>
   <si>
-    <t>Shuffle one card back into your deck, then draw 2 cards.</t>
-  </si>
-  <si>
     <t>Infiltrator</t>
   </si>
   <si>
@@ -485,6 +482,9 @@
   </si>
   <si>
     <t>Hire one Unit from your opponent's side of the field.</t>
+  </si>
+  <si>
+    <t>Shuffle one card back into your deck from your hand, then draw 2 cards.</t>
   </si>
 </sst>
 </file>
@@ -882,7 +882,7 @@
   <dimension ref="D2:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1646,7 +1646,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="4:11" x14ac:dyDescent="0.25">
@@ -1654,7 +1654,7 @@
         <v>30</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>12</v>
@@ -1669,7 +1669,7 @@
         <v>1</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="4:10" x14ac:dyDescent="0.25">
@@ -1677,7 +1677,7 @@
         <v>31</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>11</v>
@@ -1692,7 +1692,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="4:10" x14ac:dyDescent="0.25">
@@ -1700,7 +1700,7 @@
         <v>32</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>11</v>
@@ -1715,7 +1715,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="4:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implemented the SleightOfHand card
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\ce301_thorn_t\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="77">
   <si>
     <t>Card ID</t>
   </si>
@@ -490,8 +485,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -635,7 +630,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -667,10 +662,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -702,7 +696,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -878,14 +871,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D2:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="9.140625" style="7"/>
     <col min="5" max="5" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
@@ -896,7 +889,7 @@
     <col min="10" max="10" width="163.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:11">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -922,7 +915,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:11">
       <c r="D3" s="6">
         <v>1</v>
       </c>
@@ -948,7 +941,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:11">
       <c r="D4" s="6">
         <v>2</v>
       </c>
@@ -974,7 +967,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:11">
       <c r="D5" s="6">
         <v>3</v>
       </c>
@@ -1000,7 +993,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:11">
       <c r="D6" s="6">
         <v>4</v>
       </c>
@@ -1026,7 +1019,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:11">
       <c r="D7" s="6">
         <v>5</v>
       </c>
@@ -1052,7 +1045,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:11">
       <c r="D8" s="6">
         <v>6</v>
       </c>
@@ -1078,7 +1071,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:11">
       <c r="D9" s="6">
         <v>7</v>
       </c>
@@ -1104,7 +1097,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:11">
       <c r="D10" s="6">
         <v>8</v>
       </c>
@@ -1130,7 +1123,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:11">
       <c r="D11" s="7">
         <v>9</v>
       </c>
@@ -1156,7 +1149,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:11">
       <c r="D12" s="7">
         <v>10</v>
       </c>
@@ -1182,7 +1175,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:11">
       <c r="D13" s="7">
         <v>11</v>
       </c>
@@ -1208,7 +1201,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:11">
       <c r="D14" s="7">
         <v>12</v>
       </c>
@@ -1234,7 +1227,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:11">
       <c r="D15" s="7">
         <v>13</v>
       </c>
@@ -1260,7 +1253,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:11">
       <c r="D16" s="7">
         <v>14</v>
       </c>
@@ -1286,7 +1279,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:11">
       <c r="D17" s="7">
         <v>15</v>
       </c>
@@ -1312,7 +1305,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:11">
       <c r="D18" s="7">
         <v>16</v>
       </c>
@@ -1338,7 +1331,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:11">
       <c r="D19" s="7">
         <v>17</v>
       </c>
@@ -1364,7 +1357,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:11">
       <c r="D20" s="7">
         <v>18</v>
       </c>
@@ -1390,7 +1383,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:11">
       <c r="D21" s="7">
         <v>19</v>
       </c>
@@ -1416,7 +1409,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:11">
       <c r="D22" s="7">
         <v>20</v>
       </c>
@@ -1442,7 +1435,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:11">
       <c r="D23" s="7">
         <v>21</v>
       </c>
@@ -1464,8 +1457,11 @@
       <c r="J23" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="4:11">
       <c r="D24" s="7">
         <v>22</v>
       </c>
@@ -1487,8 +1483,11 @@
       <c r="J24" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="4:11">
       <c r="D25" s="7">
         <v>23</v>
       </c>
@@ -1510,8 +1509,11 @@
       <c r="J25" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11">
       <c r="D26" s="7">
         <v>24</v>
       </c>
@@ -1533,8 +1535,11 @@
       <c r="J26" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="4:11">
       <c r="D27" s="7">
         <v>25</v>
       </c>
@@ -1556,8 +1561,11 @@
       <c r="J27" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="4:11">
       <c r="D28" s="7">
         <v>26</v>
       </c>
@@ -1579,8 +1587,11 @@
       <c r="J28" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="4:11">
       <c r="D29" s="7">
         <v>27</v>
       </c>
@@ -1602,8 +1613,11 @@
       <c r="J29" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="4:11">
       <c r="D30" s="7">
         <v>28</v>
       </c>
@@ -1625,8 +1639,11 @@
       <c r="J30" s="5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="4:11">
       <c r="D31" s="7">
         <v>29</v>
       </c>
@@ -1648,8 +1665,11 @@
       <c r="J31" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="4:11">
       <c r="D32" s="7">
         <v>30</v>
       </c>
@@ -1671,8 +1691,11 @@
       <c r="J32" s="5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="4:11">
       <c r="D33" s="7">
         <v>31</v>
       </c>
@@ -1694,8 +1717,11 @@
       <c r="J33" s="5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="34" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="4:11">
       <c r="D34" s="7">
         <v>32</v>
       </c>
@@ -1717,343 +1743,346 @@
       <c r="J34" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="35" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="4:11">
       <c r="D35" s="7">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:11">
       <c r="D36" s="7">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:11">
       <c r="D37" s="7">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:11">
       <c r="D38" s="7">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:11">
       <c r="D39" s="7">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:11">
       <c r="D40" s="7">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:11">
       <c r="D41" s="7">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:11">
       <c r="D42" s="7">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:11">
       <c r="D43" s="7">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:11">
       <c r="D44" s="7">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:11">
       <c r="D45" s="7">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:11">
       <c r="D46" s="7">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:11">
       <c r="D47" s="7">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:11">
       <c r="D48" s="7">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:4">
       <c r="D49" s="7">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:4">
       <c r="D50" s="7">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:4">
       <c r="D51" s="7">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:4">
       <c r="D52" s="7">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:4">
       <c r="D53" s="7">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:4">
       <c r="D54" s="7">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:4">
       <c r="D55" s="7">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:4">
       <c r="D56" s="7">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:4">
       <c r="D57" s="7">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:4">
       <c r="D58" s="7">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:4">
       <c r="D59" s="7">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:4">
       <c r="D60" s="7">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:4">
       <c r="D61" s="7">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:4">
       <c r="D62" s="7">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:4">
       <c r="D63" s="7">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:4">
       <c r="D64" s="7">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:4">
       <c r="D65" s="7">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:4">
       <c r="D66" s="7">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:4">
       <c r="D67" s="7">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:4">
       <c r="D68" s="7">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:4">
       <c r="D69" s="7">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:4">
       <c r="D70" s="7">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:4">
       <c r="D71" s="7">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:4">
       <c r="D72" s="7">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:4">
       <c r="D73" s="7">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:4">
       <c r="D74" s="7">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:4">
       <c r="D75" s="7">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:4">
       <c r="D76" s="7">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:4">
       <c r="D77" s="7">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:4">
       <c r="D78" s="7">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:4">
       <c r="D79" s="7">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:4">
       <c r="D80" s="7">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:4">
       <c r="D81" s="7">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:4">
       <c r="D82" s="7">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:4">
       <c r="D83" s="7">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:4">
       <c r="D84" s="7">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:4">
       <c r="D85" s="7">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:4">
       <c r="D86" s="7">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:4">
       <c r="D87" s="7">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:4">
       <c r="D88" s="7">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:4">
       <c r="D89" s="7">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:4">
       <c r="D90" s="7">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:4">
       <c r="D91" s="7">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:4">
       <c r="D92" s="7">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:4">
       <c r="D93" s="7">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:4">
       <c r="D94" s="7">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:4">
       <c r="D95" s="7">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:4">
       <c r="D96" s="7">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:4">
       <c r="D97" s="7">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:4">
       <c r="D98" s="7">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:4">
       <c r="D99" s="7">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:4">
       <c r="D100" s="7">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:4">
       <c r="D101" s="7">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:4">
       <c r="D102" s="7">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Renamed Illusionary Frog to Illusion Frog
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -326,9 +326,6 @@
     <t>When this minion is killed, you can bury it instead. When this minion is ressurected, its strength and health becomes 7.</t>
   </si>
   <si>
-    <t>Illusionary frog</t>
-  </si>
-  <si>
     <t>Bloated Body</t>
   </si>
   <si>
@@ -480,6 +477,9 @@
   </si>
   <si>
     <t>Shuffle one card back into your deck from your hand, then draw 2 cards.</t>
+  </si>
+  <si>
+    <t>Illusion frog</t>
   </si>
 </sst>
 </file>
@@ -875,7 +875,7 @@
   <dimension ref="D2:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1091,7 +1091,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K9" t="s">
         <v>44</v>
@@ -1117,7 +1117,7 @@
         <v>5</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K10" t="s">
         <v>44</v>
@@ -1143,7 +1143,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K11" t="s">
         <v>44</v>
@@ -1169,7 +1169,7 @@
         <v>2</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K12" t="s">
         <v>44</v>
@@ -1387,8 +1387,8 @@
       <c r="D21" s="7">
         <v>19</v>
       </c>
-      <c r="E21" s="8" t="s">
-        <v>60</v>
+      <c r="E21" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>12</v>
@@ -1403,7 +1403,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K21" t="s">
         <v>44</v>
@@ -1585,7 +1585,7 @@
         <v>2</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K28" t="s">
         <v>44</v>
@@ -1622,7 +1622,7 @@
         <v>28</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>12</v>
@@ -1637,7 +1637,7 @@
         <v>1</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K30" t="s">
         <v>44</v>
@@ -1648,7 +1648,7 @@
         <v>29</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>11</v>
@@ -1663,7 +1663,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K31" t="s">
         <v>43</v>
@@ -1674,7 +1674,7 @@
         <v>30</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>12</v>
@@ -1689,7 +1689,7 @@
         <v>1</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K32" t="s">
         <v>44</v>
@@ -1700,7 +1700,7 @@
         <v>31</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>11</v>
@@ -1715,7 +1715,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K33" t="s">
         <v>44</v>
@@ -1726,7 +1726,7 @@
         <v>32</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>11</v>
@@ -1741,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K34" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
Implemented the 'Dying Nobleman' card
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\ce301_thorn_t\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075"/>
   </bookViews>
@@ -485,8 +490,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -630,7 +635,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -662,9 +667,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -696,6 +702,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -871,14 +878,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C11" activeCellId="1" sqref="I18 C11"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="9.140625" style="7"/>
     <col min="5" max="5" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
@@ -889,7 +896,7 @@
     <col min="10" max="10" width="163.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:11">
+    <row r="2" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -915,7 +922,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="4:11">
+    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D3" s="6">
         <v>1</v>
       </c>
@@ -941,7 +948,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="4:11">
+    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D4" s="6">
         <v>2</v>
       </c>
@@ -967,7 +974,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="4:11">
+    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D5" s="6">
         <v>3</v>
       </c>
@@ -993,7 +1000,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="4:11">
+    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D6" s="6">
         <v>4</v>
       </c>
@@ -1019,7 +1026,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="4:11">
+    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D7" s="6">
         <v>5</v>
       </c>
@@ -1045,7 +1052,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="4:11">
+    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D8" s="6">
         <v>6</v>
       </c>
@@ -1071,7 +1078,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="4:11">
+    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D9" s="6">
         <v>7</v>
       </c>
@@ -1097,7 +1104,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="4:11">
+    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D10" s="6">
         <v>8</v>
       </c>
@@ -1123,7 +1130,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="4:11">
+    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D11" s="7">
         <v>9</v>
       </c>
@@ -1149,7 +1156,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="4:11">
+    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D12" s="7">
         <v>10</v>
       </c>
@@ -1175,7 +1182,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="4:11">
+    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D13" s="7">
         <v>11</v>
       </c>
@@ -1201,7 +1208,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="4:11">
+    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D14" s="7">
         <v>12</v>
       </c>
@@ -1227,7 +1234,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="4:11">
+    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D15" s="7">
         <v>13</v>
       </c>
@@ -1253,7 +1260,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="4:11">
+    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D16" s="7">
         <v>14</v>
       </c>
@@ -1279,7 +1286,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="4:11">
+    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D17" s="7">
         <v>15</v>
       </c>
@@ -1305,7 +1312,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="4:11">
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D18" s="7">
         <v>16</v>
       </c>
@@ -1328,10 +1335,10 @@
         <v>38</v>
       </c>
       <c r="K18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="4:11">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D19" s="7">
         <v>17</v>
       </c>
@@ -1357,7 +1364,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="4:11">
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D20" s="7">
         <v>18</v>
       </c>
@@ -1383,7 +1390,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="4:11">
+    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D21" s="7">
         <v>19</v>
       </c>
@@ -1409,7 +1416,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="4:11">
+    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D22" s="7">
         <v>20</v>
       </c>
@@ -1435,7 +1442,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="4:11">
+    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D23" s="7">
         <v>21</v>
       </c>
@@ -1461,7 +1468,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="4:11">
+    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D24" s="7">
         <v>22</v>
       </c>
@@ -1487,7 +1494,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="4:11">
+    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D25" s="7">
         <v>23</v>
       </c>
@@ -1513,7 +1520,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="4:11">
+    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D26" s="7">
         <v>24</v>
       </c>
@@ -1539,7 +1546,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="4:11">
+    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D27" s="7">
         <v>25</v>
       </c>
@@ -1565,7 +1572,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="4:11">
+    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D28" s="7">
         <v>26</v>
       </c>
@@ -1591,7 +1598,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="4:11">
+    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D29" s="7">
         <v>27</v>
       </c>
@@ -1617,7 +1624,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="4:11">
+    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D30" s="7">
         <v>28</v>
       </c>
@@ -1643,7 +1650,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="4:11">
+    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D31" s="7">
         <v>29</v>
       </c>
@@ -1669,7 +1676,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="4:11">
+    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D32" s="7">
         <v>30</v>
       </c>
@@ -1695,7 +1702,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="4:11">
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D33" s="7">
         <v>31</v>
       </c>
@@ -1721,7 +1728,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="4:11">
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D34" s="7">
         <v>32</v>
       </c>
@@ -1747,342 +1754,342 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="4:11">
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D35" s="7">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="4:11">
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D36" s="7">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="4:11">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="7">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="4:11">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="7">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="4:11">
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="7">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="4:11">
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="7">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="4:11">
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="7">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="4:11">
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="7">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="4:11">
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="7">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="4:11">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="7">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="4:11">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="7">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="4:11">
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="7">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="4:11">
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="7">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="4:11">
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="7">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="4:4">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="7">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="4:4">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="7">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="4:4">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="7">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="4:4">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="7">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="4:4">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="7">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="4:4">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="7">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="4:4">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" s="7">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="4:4">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" s="7">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="4:4">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" s="7">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="4:4">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D58" s="7">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="4:4">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D59" s="7">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="4:4">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D60" s="7">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="4:4">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D61" s="7">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="4:4">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D62" s="7">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="4:4">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D63" s="7">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="4:4">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D64" s="7">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="4:4">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" s="7">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="4:4">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="7">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="4:4">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" s="7">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="4:4">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" s="7">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="4:4">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D69" s="7">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="4:4">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D70" s="7">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="4:4">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D71" s="7">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="4:4">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D72" s="7">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="4:4">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D73" s="7">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="4:4">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D74" s="7">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="4:4">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D75" s="7">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="4:4">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D76" s="7">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="4:4">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D77" s="7">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="4:4">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D78" s="7">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="4:4">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D79" s="7">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="4:4">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D80" s="7">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="4:4">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D81" s="7">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="4:4">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D82" s="7">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="4:4">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D83" s="7">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="4:4">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D84" s="7">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="4:4">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D85" s="7">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="4:4">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D86" s="7">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="4:4">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D87" s="7">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="4:4">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D88" s="7">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="4:4">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D89" s="7">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="4:4">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D90" s="7">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="4:4">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D91" s="7">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="4:4">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D92" s="7">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="4:4">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D93" s="7">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="4:4">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D94" s="7">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="4:4">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D95" s="7">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="4:4">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D96" s="7">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="4:4">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D97" s="7">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="4:4">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D98" s="7">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="4:4">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D99" s="7">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="4:4">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D100" s="7">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="4:4">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D101" s="7">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="4:4">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D102" s="7">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Created the 'Illusion Frog' card
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -882,7 +882,7 @@
   <dimension ref="D2:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1413,7 +1413,7 @@
         <v>65</v>
       </c>
       <c r="K21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implemented the 'Bloated Body' Card
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -881,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1647,7 +1647,7 @@
         <v>61</v>
       </c>
       <c r="K30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="4:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed the Dropzone tags on deck builder zones
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -881,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,7 +1049,7 @@
         <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="4:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Renamed some cards, buffed Withdrawal (now called Trinkets & Baubles) to give 5 gold.
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -229,12 +229,6 @@
     <t>If this card defeats an opponents minion in battle, you can pay 1 coin bury it to your side of the battlefield.</t>
   </si>
   <si>
-    <t>Withdrawal</t>
-  </si>
-  <si>
-    <t>Gain 2 gold.</t>
-  </si>
-  <si>
     <t>Lucky Dip</t>
   </si>
   <si>
@@ -244,15 +238,9 @@
     <t>Occult Devotee</t>
   </si>
   <si>
-    <t>Eldrich Horror</t>
-  </si>
-  <si>
     <t>If you control 5 occult devotees, call upon an "Eldrich Horror" from your hand, deck, or discard pile.</t>
   </si>
   <si>
-    <t>Reusable tools</t>
-  </si>
-  <si>
     <t>Return a Utility in your discard pile to your hand</t>
   </si>
   <si>
@@ -469,9 +457,6 @@
     <t>When you hire this card, kill one Unit on your opponent's side of the field, then switch control of this card.</t>
   </si>
   <si>
-    <t>Artillery</t>
-  </si>
-  <si>
     <t>Treachary</t>
   </si>
   <si>
@@ -485,6 +470,21 @@
   </si>
   <si>
     <t>Illusion frog</t>
+  </si>
+  <si>
+    <t>Gain 5 gold.</t>
+  </si>
+  <si>
+    <t>Trinkets and Baubles</t>
+  </si>
+  <si>
+    <t>Eldritch Horror</t>
+  </si>
+  <si>
+    <t>Rain of Fire</t>
+  </si>
+  <si>
+    <t>Desperate Times</t>
   </si>
 </sst>
 </file>
@@ -882,13 +882,13 @@
   <dimension ref="D2:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="9.140625" style="7"/>
-    <col min="5" max="5" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
@@ -919,7 +919,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="4:11" x14ac:dyDescent="0.25">
@@ -945,7 +945,7 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="4:11" x14ac:dyDescent="0.25">
@@ -971,7 +971,7 @@
         <v>20</v>
       </c>
       <c r="K4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="4:11" x14ac:dyDescent="0.25">
@@ -997,7 +997,7 @@
         <v>19</v>
       </c>
       <c r="K5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="4:11" x14ac:dyDescent="0.25">
@@ -1023,7 +1023,7 @@
         <v>18</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="4:11" x14ac:dyDescent="0.25">
@@ -1049,7 +1049,7 @@
         <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="4:11" x14ac:dyDescent="0.25">
@@ -1075,7 +1075,7 @@
         <v>25</v>
       </c>
       <c r="K8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="4:11" x14ac:dyDescent="0.25">
@@ -1098,10 +1098,10 @@
         <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="K9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="4:11" x14ac:dyDescent="0.25">
@@ -1124,10 +1124,10 @@
         <v>5</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="4:11" x14ac:dyDescent="0.25">
@@ -1150,10 +1150,10 @@
         <v>1</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="K11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="4:11" x14ac:dyDescent="0.25">
@@ -1176,10 +1176,10 @@
         <v>2</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="K12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="4:11" x14ac:dyDescent="0.25">
@@ -1187,7 +1187,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>11</v>
@@ -1202,10 +1202,10 @@
         <v>0</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="K13" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="4:11" x14ac:dyDescent="0.25">
@@ -1213,7 +1213,7 @@
         <v>12</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>11</v>
@@ -1228,10 +1228,10 @@
         <v>0</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="4:11" x14ac:dyDescent="0.25">
@@ -1239,7 +1239,7 @@
         <v>13</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>12</v>
@@ -1254,10 +1254,10 @@
         <v>2</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="4:11" x14ac:dyDescent="0.25">
@@ -1265,7 +1265,7 @@
         <v>14</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>12</v>
@@ -1280,10 +1280,10 @@
         <v>30</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
@@ -1291,7 +1291,7 @@
         <v>15</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>11</v>
@@ -1306,10 +1306,10 @@
         <v>0</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="K17" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.25">
@@ -1317,7 +1317,7 @@
         <v>16</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>12</v>
@@ -1332,10 +1332,10 @@
         <v>1</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="K18" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.25">
@@ -1343,7 +1343,7 @@
         <v>17</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>12</v>
@@ -1358,10 +1358,10 @@
         <v>3</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K19" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.25">
@@ -1369,7 +1369,7 @@
         <v>18</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>12</v>
@@ -1384,10 +1384,10 @@
         <v>5</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K20" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.25">
@@ -1395,7 +1395,7 @@
         <v>19</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>12</v>
@@ -1410,10 +1410,10 @@
         <v>2</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="K21" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.25">
@@ -1421,7 +1421,7 @@
         <v>20</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>11</v>
@@ -1436,10 +1436,10 @@
         <v>0</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="K22" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="4:11" x14ac:dyDescent="0.25">
@@ -1447,7 +1447,7 @@
         <v>21</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>12</v>
@@ -1462,10 +1462,10 @@
         <v>1</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K23" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="4:11" x14ac:dyDescent="0.25">
@@ -1473,7 +1473,7 @@
         <v>22</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>12</v>
@@ -1488,10 +1488,10 @@
         <v>2</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="K24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="4:11" x14ac:dyDescent="0.25">
@@ -1499,7 +1499,7 @@
         <v>23</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>11</v>
@@ -1514,10 +1514,10 @@
         <v>0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="K25" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="4:11" x14ac:dyDescent="0.25">
@@ -1525,7 +1525,7 @@
         <v>24</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>11</v>
@@ -1540,10 +1540,10 @@
         <v>0</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="K26" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="4:11" x14ac:dyDescent="0.25">
@@ -1551,7 +1551,7 @@
         <v>25</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>12</v>
@@ -1566,10 +1566,10 @@
         <v>1</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="K27" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="4:11" x14ac:dyDescent="0.25">
@@ -1577,7 +1577,7 @@
         <v>26</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>12</v>
@@ -1592,10 +1592,10 @@
         <v>2</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="K28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="4:11" x14ac:dyDescent="0.25">
@@ -1603,7 +1603,7 @@
         <v>27</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>11</v>
@@ -1618,10 +1618,10 @@
         <v>0</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="K29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="4:11" x14ac:dyDescent="0.25">
@@ -1629,7 +1629,7 @@
         <v>28</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>12</v>
@@ -1644,10 +1644,10 @@
         <v>1</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K30" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="4:11" x14ac:dyDescent="0.25">
@@ -1655,7 +1655,7 @@
         <v>29</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>11</v>
@@ -1670,10 +1670,10 @@
         <v>0</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="K31" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="4:11" x14ac:dyDescent="0.25">
@@ -1681,7 +1681,7 @@
         <v>30</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>12</v>
@@ -1696,10 +1696,10 @@
         <v>1</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K32" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="4:11" x14ac:dyDescent="0.25">
@@ -1707,7 +1707,7 @@
         <v>31</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>11</v>
@@ -1722,10 +1722,10 @@
         <v>0</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="K33" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="4:11" x14ac:dyDescent="0.25">
@@ -1733,7 +1733,7 @@
         <v>32</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>11</v>
@@ -1748,10 +1748,10 @@
         <v>0</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="K34" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="4:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Made some changes to the wording on Combat Medic
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -286,9 +286,6 @@
     <t>Combat Medic</t>
   </si>
   <si>
-    <t>When this minion is summoned, you can restore 2 health to a minion on the field. You can pay 2 gold, restore 2 health to a minion on the field.</t>
-  </si>
-  <si>
     <t>Immunity</t>
   </si>
   <si>
@@ -485,6 +482,9 @@
   </si>
   <si>
     <t>Desperate Times</t>
+  </si>
+  <si>
+    <t>When this minion is summoned, you can restore 2 health to a minion on the field. Once per turn, you can pay 2 gold, restore 2 health to a minion on the field.</t>
   </si>
 </sst>
 </file>
@@ -882,7 +882,7 @@
   <dimension ref="D2:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,7 +1098,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K9" t="s">
         <v>40</v>
@@ -1124,7 +1124,7 @@
         <v>5</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K10" t="s">
         <v>40</v>
@@ -1150,7 +1150,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K11" t="s">
         <v>40</v>
@@ -1176,7 +1176,7 @@
         <v>2</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K12" t="s">
         <v>40</v>
@@ -1187,7 +1187,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>11</v>
@@ -1202,7 +1202,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K13" t="s">
         <v>39</v>
@@ -1265,7 +1265,7 @@
         <v>14</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>12</v>
@@ -1291,7 +1291,7 @@
         <v>15</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>11</v>
@@ -1384,7 +1384,7 @@
         <v>5</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K20" t="s">
         <v>40</v>
@@ -1395,7 +1395,7 @@
         <v>19</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>12</v>
@@ -1410,7 +1410,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K21" t="s">
         <v>39</v>
@@ -1439,7 +1439,7 @@
         <v>37</v>
       </c>
       <c r="K22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="4:11" x14ac:dyDescent="0.25">
@@ -1488,7 +1488,7 @@
         <v>2</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="K24" t="s">
         <v>40</v>
@@ -1499,7 +1499,7 @@
         <v>23</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>11</v>
@@ -1514,7 +1514,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K25" t="s">
         <v>40</v>
@@ -1525,7 +1525,7 @@
         <v>24</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>11</v>
@@ -1540,7 +1540,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K26" t="s">
         <v>40</v>
@@ -1551,7 +1551,7 @@
         <v>25</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>12</v>
@@ -1566,7 +1566,7 @@
         <v>1</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K27" t="s">
         <v>40</v>
@@ -1577,7 +1577,7 @@
         <v>26</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>12</v>
@@ -1592,7 +1592,7 @@
         <v>2</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K28" t="s">
         <v>40</v>
@@ -1603,7 +1603,7 @@
         <v>27</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>11</v>
@@ -1618,7 +1618,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K29" t="s">
         <v>40</v>
@@ -1629,7 +1629,7 @@
         <v>28</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>12</v>
@@ -1644,7 +1644,7 @@
         <v>1</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K30" t="s">
         <v>39</v>
@@ -1655,7 +1655,7 @@
         <v>29</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>11</v>
@@ -1670,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K31" t="s">
         <v>39</v>
@@ -1681,7 +1681,7 @@
         <v>30</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>12</v>
@@ -1696,7 +1696,7 @@
         <v>1</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K32" t="s">
         <v>40</v>
@@ -1707,7 +1707,7 @@
         <v>31</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>11</v>
@@ -1722,7 +1722,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K33" t="s">
         <v>40</v>
@@ -1733,7 +1733,7 @@
         <v>32</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>11</v>
@@ -1748,7 +1748,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K34" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Create the 'Negotiator' card
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -301,9 +301,6 @@
     <t>Negotiator</t>
   </si>
   <si>
-    <t>While this unit is on the field - you do not pay wages for your units.</t>
-  </si>
-  <si>
     <t>Toxic Frog</t>
   </si>
   <si>
@@ -485,6 +482,9 @@
   </si>
   <si>
     <t>When this minion is summoned, you can restore 2 health to a minion on the field. Once per turn, you can pay 2 gold, restore 2 health to a minion on the field.</t>
+  </si>
+  <si>
+    <t>While this unit is on the field, you do not pay wages for your units.</t>
   </si>
 </sst>
 </file>
@@ -881,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,7 +1098,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K9" t="s">
         <v>40</v>
@@ -1124,7 +1124,7 @@
         <v>5</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K10" t="s">
         <v>40</v>
@@ -1150,7 +1150,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K11" t="s">
         <v>40</v>
@@ -1176,7 +1176,7 @@
         <v>2</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K12" t="s">
         <v>40</v>
@@ -1187,7 +1187,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>11</v>
@@ -1202,7 +1202,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K13" t="s">
         <v>39</v>
@@ -1265,7 +1265,7 @@
         <v>14</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>12</v>
@@ -1291,7 +1291,7 @@
         <v>15</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>11</v>
@@ -1384,7 +1384,7 @@
         <v>5</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K20" t="s">
         <v>40</v>
@@ -1395,7 +1395,7 @@
         <v>19</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>12</v>
@@ -1410,7 +1410,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K21" t="s">
         <v>39</v>
@@ -1488,7 +1488,7 @@
         <v>2</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K24" t="s">
         <v>40</v>
@@ -1566,10 +1566,10 @@
         <v>1</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="K27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="4:11" x14ac:dyDescent="0.25">
@@ -1577,7 +1577,7 @@
         <v>26</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>12</v>
@@ -1592,7 +1592,7 @@
         <v>2</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K28" t="s">
         <v>40</v>
@@ -1603,7 +1603,7 @@
         <v>27</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>11</v>
@@ -1618,7 +1618,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K29" t="s">
         <v>40</v>
@@ -1629,7 +1629,7 @@
         <v>28</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>12</v>
@@ -1644,7 +1644,7 @@
         <v>1</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K30" t="s">
         <v>39</v>
@@ -1655,7 +1655,7 @@
         <v>29</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>11</v>
@@ -1670,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K31" t="s">
         <v>39</v>
@@ -1681,7 +1681,7 @@
         <v>30</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>12</v>
@@ -1696,7 +1696,7 @@
         <v>1</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K32" t="s">
         <v>40</v>
@@ -1707,7 +1707,7 @@
         <v>31</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>11</v>
@@ -1722,7 +1722,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K33" t="s">
         <v>40</v>
@@ -1733,7 +1733,7 @@
         <v>32</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>11</v>
@@ -1748,7 +1748,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K34" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Implemented the Combat Medic card
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -469,9 +469,6 @@
     <t>Gain 5 gold.</t>
   </si>
   <si>
-    <t>Trinkets and Baubles</t>
-  </si>
-  <si>
     <t>Eldritch Horror</t>
   </si>
   <si>
@@ -481,10 +478,13 @@
     <t>Desperate Times</t>
   </si>
   <si>
-    <t>When this minion is summoned, you can restore 2 health to a minion on the field. Once per turn, you can pay 2 gold, restore 2 health to a minion on the field.</t>
-  </si>
-  <si>
     <t>While this unit is on the field, you do not pay wages for your units.</t>
+  </si>
+  <si>
+    <t>Trinkets &amp; Baubles</t>
+  </si>
+  <si>
+    <t>Once per turn, you can pay 1 gold, restore 2 health to a unit on the field.</t>
   </si>
 </sst>
 </file>
@@ -882,7 +882,7 @@
   <dimension ref="D2:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1187,7 +1187,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>11</v>
@@ -1265,7 +1265,7 @@
         <v>14</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>12</v>
@@ -1291,7 +1291,7 @@
         <v>15</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>11</v>
@@ -1488,10 +1488,10 @@
         <v>2</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="4:11" x14ac:dyDescent="0.25">
@@ -1566,7 +1566,7 @@
         <v>1</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K27" t="s">
         <v>39</v>
@@ -1707,7 +1707,7 @@
         <v>31</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Added a method to search cards from deck by name
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\ce301_thorn_t\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075"/>
   </bookViews>
@@ -223,9 +218,6 @@
     <t>Sticky Tongue Frog</t>
   </si>
   <si>
-    <t>Friendship Frog</t>
-  </si>
-  <si>
     <t>If this card defeats an opponents minion in battle, you can pay 1 coin bury it to your side of the battlefield.</t>
   </si>
   <si>
@@ -368,6 +360,102 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">When this minion reaches 0 health from combat, you can </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">bounce </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>this unit instead of killing it.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">You can </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">bounce </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>this unit, place 3 poison counters on an enemy unit.</t>
+    </r>
+  </si>
+  <si>
+    <t>Send a buried minion to it's owner's Discard Pile.</t>
+  </si>
+  <si>
+    <t>Sleight of Hand</t>
+  </si>
+  <si>
+    <t>Infiltrator</t>
+  </si>
+  <si>
+    <t>When you hire this card, kill one Unit on your opponent's side of the field, then switch control of this card.</t>
+  </si>
+  <si>
+    <t>Treachary</t>
+  </si>
+  <si>
+    <t>Deal 2 damage to all Minions your opponent controls.</t>
+  </si>
+  <si>
+    <t>Hire one Unit from your opponent's side of the field.</t>
+  </si>
+  <si>
+    <t>Shuffle one card back into your deck from your hand, then draw 2 cards.</t>
+  </si>
+  <si>
+    <t>Illusion frog</t>
+  </si>
+  <si>
+    <t>Gain 5 gold.</t>
+  </si>
+  <si>
+    <t>Eldritch Horror</t>
+  </si>
+  <si>
+    <t>Rain of Fire</t>
+  </si>
+  <si>
+    <t>Desperate Times</t>
+  </si>
+  <si>
+    <t>While this unit is on the field, you do not pay wages for your units.</t>
+  </si>
+  <si>
+    <t>Trinkets &amp; Baubles</t>
+  </si>
+  <si>
+    <t>Once per turn, you can pay 1 gold, restore 2 health to a unit on the field.</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">You can pay 3 coins, </t>
     </r>
     <r>
@@ -387,111 +475,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> this unit, then you can add 1 "Frog" card to your hand, from your deck.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">When this minion reaches 0 health from combat, you can </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">bounce </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>this unit instead of killing it.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">You can </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">bounce </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>this unit, place 3 poison counters on an enemy unit.</t>
-    </r>
-  </si>
-  <si>
-    <t>Send a buried minion to it's owner's Discard Pile.</t>
-  </si>
-  <si>
-    <t>Sleight of Hand</t>
-  </si>
-  <si>
-    <t>Infiltrator</t>
-  </si>
-  <si>
-    <t>When you hire this card, kill one Unit on your opponent's side of the field, then switch control of this card.</t>
-  </si>
-  <si>
-    <t>Treachary</t>
-  </si>
-  <si>
-    <t>Deal 2 damage to all Minions your opponent controls.</t>
-  </si>
-  <si>
-    <t>Hire one Unit from your opponent's side of the field.</t>
-  </si>
-  <si>
-    <t>Shuffle one card back into your deck from your hand, then draw 2 cards.</t>
-  </si>
-  <si>
-    <t>Illusion frog</t>
-  </si>
-  <si>
-    <t>Gain 5 gold.</t>
-  </si>
-  <si>
-    <t>Eldritch Horror</t>
-  </si>
-  <si>
-    <t>Rain of Fire</t>
-  </si>
-  <si>
-    <t>Desperate Times</t>
-  </si>
-  <si>
-    <t>While this unit is on the field, you do not pay wages for your units.</t>
-  </si>
-  <si>
-    <t>Trinkets &amp; Baubles</t>
-  </si>
-  <si>
-    <t>Once per turn, you can pay 1 gold, restore 2 health to a unit on the field.</t>
+      <t xml:space="preserve"> this unit, then add 1 "Frog" card from your deck to your hand.</t>
+    </r>
+  </si>
+  <si>
+    <t>Frog Elder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -635,7 +630,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -667,10 +662,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -702,7 +696,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -878,14 +871,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D2:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="9.140625" style="7"/>
     <col min="5" max="5" width="19.5703125" style="10" bestFit="1" customWidth="1"/>
@@ -896,7 +889,7 @@
     <col min="10" max="10" width="163.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:11">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -919,10 +912,10 @@
         <v>3</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="4:11">
       <c r="D3" s="6">
         <v>1</v>
       </c>
@@ -945,10 +938,10 @@
         <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="4:11">
       <c r="D4" s="6">
         <v>2</v>
       </c>
@@ -971,10 +964,10 @@
         <v>20</v>
       </c>
       <c r="K4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="4:11">
       <c r="D5" s="6">
         <v>3</v>
       </c>
@@ -997,10 +990,10 @@
         <v>19</v>
       </c>
       <c r="K5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="4:11">
       <c r="D6" s="6">
         <v>4</v>
       </c>
@@ -1023,10 +1016,10 @@
         <v>18</v>
       </c>
       <c r="K6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="4:11">
       <c r="D7" s="6">
         <v>5</v>
       </c>
@@ -1049,10 +1042,10 @@
         <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="4:11">
       <c r="D8" s="6">
         <v>6</v>
       </c>
@@ -1072,13 +1065,13 @@
         <v>2</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="4:11">
       <c r="D9" s="6">
         <v>7</v>
       </c>
@@ -1098,13 +1091,13 @@
         <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="4:11">
       <c r="D10" s="6">
         <v>8</v>
       </c>
@@ -1124,13 +1117,13 @@
         <v>5</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="4:11">
       <c r="D11" s="7">
         <v>9</v>
       </c>
@@ -1150,18 +1143,18 @@
         <v>1</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="4:11">
       <c r="D12" s="7">
         <v>10</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>24</v>
+      <c r="E12" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>12</v>
@@ -1176,18 +1169,18 @@
         <v>2</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="K12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="4:11">
       <c r="D13" s="7">
         <v>11</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>11</v>
@@ -1202,18 +1195,18 @@
         <v>0</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="4:11">
       <c r="D14" s="7">
         <v>12</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>11</v>
@@ -1228,18 +1221,18 @@
         <v>0</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11">
       <c r="D15" s="7">
         <v>13</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>12</v>
@@ -1254,18 +1247,18 @@
         <v>2</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="4:11">
       <c r="D16" s="7">
         <v>14</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>12</v>
@@ -1280,18 +1273,18 @@
         <v>30</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11">
       <c r="D17" s="7">
         <v>15</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>11</v>
@@ -1306,18 +1299,18 @@
         <v>0</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11">
       <c r="D18" s="7">
         <v>16</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>12</v>
@@ -1332,18 +1325,18 @@
         <v>1</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11">
       <c r="D19" s="7">
         <v>17</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>12</v>
@@ -1358,18 +1351,18 @@
         <v>3</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11">
       <c r="D20" s="7">
         <v>18</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>12</v>
@@ -1384,18 +1377,18 @@
         <v>5</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11">
       <c r="D21" s="7">
         <v>19</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>12</v>
@@ -1410,18 +1403,18 @@
         <v>2</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11">
       <c r="D22" s="7">
         <v>20</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>11</v>
@@ -1436,18 +1429,18 @@
         <v>0</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11">
       <c r="D23" s="7">
         <v>21</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>12</v>
@@ -1462,18 +1455,18 @@
         <v>1</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="4:11">
       <c r="D24" s="7">
         <v>22</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>12</v>
@@ -1488,18 +1481,18 @@
         <v>2</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="4:11">
       <c r="D25" s="7">
         <v>23</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>11</v>
@@ -1514,18 +1507,18 @@
         <v>0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11">
       <c r="D26" s="7">
         <v>24</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>11</v>
@@ -1540,18 +1533,18 @@
         <v>0</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="4:11">
       <c r="D27" s="7">
         <v>25</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>12</v>
@@ -1566,18 +1559,18 @@
         <v>1</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="4:11">
       <c r="D28" s="7">
         <v>26</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>12</v>
@@ -1592,18 +1585,18 @@
         <v>2</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K28" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="4:11">
       <c r="D29" s="7">
         <v>27</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>11</v>
@@ -1618,18 +1611,18 @@
         <v>0</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K29" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="4:11">
       <c r="D30" s="7">
         <v>28</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>12</v>
@@ -1644,18 +1637,18 @@
         <v>1</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="4:11">
       <c r="D31" s="7">
         <v>29</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>11</v>
@@ -1670,18 +1663,18 @@
         <v>0</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="4:11">
       <c r="D32" s="7">
         <v>30</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>12</v>
@@ -1696,18 +1689,18 @@
         <v>1</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="4:11">
       <c r="D33" s="7">
         <v>31</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>11</v>
@@ -1722,18 +1715,18 @@
         <v>0</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K33" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="4:11">
       <c r="D34" s="7">
         <v>32</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>11</v>
@@ -1748,348 +1741,348 @@
         <v>0</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K34" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="4:11">
       <c r="D35" s="7">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:11">
       <c r="D36" s="7">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:11">
       <c r="D37" s="7">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:11">
       <c r="D38" s="7">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:11">
       <c r="D39" s="7">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:11">
       <c r="D40" s="7">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:11">
       <c r="D41" s="7">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:11">
       <c r="D42" s="7">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:11">
       <c r="D43" s="7">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:11">
       <c r="D44" s="7">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:11">
       <c r="D45" s="7">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:11">
       <c r="D46" s="7">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:11">
       <c r="D47" s="7">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:11">
       <c r="D48" s="7">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:4">
       <c r="D49" s="7">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:4">
       <c r="D50" s="7">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:4">
       <c r="D51" s="7">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:4">
       <c r="D52" s="7">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:4">
       <c r="D53" s="7">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:4">
       <c r="D54" s="7">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:4">
       <c r="D55" s="7">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:4">
       <c r="D56" s="7">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:4">
       <c r="D57" s="7">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:4">
       <c r="D58" s="7">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:4">
       <c r="D59" s="7">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:4">
       <c r="D60" s="7">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:4">
       <c r="D61" s="7">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:4">
       <c r="D62" s="7">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:4">
       <c r="D63" s="7">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:4">
       <c r="D64" s="7">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:4">
       <c r="D65" s="7">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:4">
       <c r="D66" s="7">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:4">
       <c r="D67" s="7">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:4">
       <c r="D68" s="7">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:4">
       <c r="D69" s="7">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:4">
       <c r="D70" s="7">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:4">
       <c r="D71" s="7">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:4">
       <c r="D72" s="7">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:4">
       <c r="D73" s="7">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:4">
       <c r="D74" s="7">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:4">
       <c r="D75" s="7">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:4">
       <c r="D76" s="7">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:4">
       <c r="D77" s="7">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:4">
       <c r="D78" s="7">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:4">
       <c r="D79" s="7">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:4">
       <c r="D80" s="7">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:4">
       <c r="D81" s="7">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:4">
       <c r="D82" s="7">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:4">
       <c r="D83" s="7">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:4">
       <c r="D84" s="7">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:4">
       <c r="D85" s="7">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:4">
       <c r="D86" s="7">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:4">
       <c r="D87" s="7">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:4">
       <c r="D88" s="7">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:4">
       <c r="D89" s="7">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:4">
       <c r="D90" s="7">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:4">
       <c r="D91" s="7">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:4">
       <c r="D92" s="7">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:4">
       <c r="D93" s="7">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:4">
       <c r="D94" s="7">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:4">
       <c r="D95" s="7">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:4">
       <c r="D96" s="7">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:4">
       <c r="D97" s="7">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:4">
       <c r="D98" s="7">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:4">
       <c r="D99" s="7">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:4">
       <c r="D100" s="7">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:4">
       <c r="D101" s="7">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:4">
       <c r="D102" s="7">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Created the Frog Elder card, giving the ability to search for cards
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -455,6 +455,9 @@
     <t>Once per turn, you can pay 1 gold, restore 2 health to a unit on the field.</t>
   </si>
   <si>
+    <t>Frog Elder</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">You can pay 3 coins, </t>
     </r>
@@ -475,11 +478,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> this unit, then add 1 "Frog" card from your deck to your hand.</t>
-    </r>
-  </si>
-  <si>
-    <t>Frog Elder</t>
+      <t xml:space="preserve"> this unit, then search 1 "Frog" card.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -874,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D2:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1154,13 +1154,13 @@
         <v>10</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="G12" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H12" s="4">
         <v>2</v>
@@ -1169,7 +1169,7 @@
         <v>2</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K12" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Updated the spreadsheet to indicate Frog Elder was done
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -874,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D2:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1172,7 +1172,7 @@
         <v>76</v>
       </c>
       <c r="K12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="4:11">

</xml_diff>

<commit_message>
Sleight Of Hand now works server-side
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -875,7 +875,7 @@
   <dimension ref="D2:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1472,7 +1472,7 @@
         <v>12</v>
       </c>
       <c r="G24" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H24" s="4">
         <v>2</v>

</xml_diff>

<commit_message>
Illlusion frog no longer optional, also handled server side
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -360,7 +360,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">When this minion reaches 0 health from combat, you can </t>
+      <t xml:space="preserve">You can </t>
     </r>
     <r>
       <rPr>
@@ -379,106 +379,106 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>this unit, place 3 poison counters on an enemy unit.</t>
+    </r>
+  </si>
+  <si>
+    <t>Send a buried minion to it's owner's Discard Pile.</t>
+  </si>
+  <si>
+    <t>Sleight of Hand</t>
+  </si>
+  <si>
+    <t>Infiltrator</t>
+  </si>
+  <si>
+    <t>When you hire this card, kill one Unit on your opponent's side of the field, then switch control of this card.</t>
+  </si>
+  <si>
+    <t>Treachary</t>
+  </si>
+  <si>
+    <t>Deal 2 damage to all Minions your opponent controls.</t>
+  </si>
+  <si>
+    <t>Hire one Unit from your opponent's side of the field.</t>
+  </si>
+  <si>
+    <t>Shuffle one card back into your deck from your hand, then draw 2 cards.</t>
+  </si>
+  <si>
+    <t>Illusion frog</t>
+  </si>
+  <si>
+    <t>Gain 5 gold.</t>
+  </si>
+  <si>
+    <t>Eldritch Horror</t>
+  </si>
+  <si>
+    <t>Rain of Fire</t>
+  </si>
+  <si>
+    <t>Desperate Times</t>
+  </si>
+  <si>
+    <t>While this unit is on the field, you do not pay wages for your units.</t>
+  </si>
+  <si>
+    <t>Trinkets &amp; Baubles</t>
+  </si>
+  <si>
+    <t>Once per turn, you can pay 1 gold, restore 2 health to a unit on the field.</t>
+  </si>
+  <si>
+    <t>Frog Elder</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">You can pay 3 coins, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bounce</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> this unit, then search 1 "Frog" card.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When this minion reaches 0 health from combat, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">bounce </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>this unit instead of killing it.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">You can </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">bounce </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>this unit, place 3 poison counters on an enemy unit.</t>
-    </r>
-  </si>
-  <si>
-    <t>Send a buried minion to it's owner's Discard Pile.</t>
-  </si>
-  <si>
-    <t>Sleight of Hand</t>
-  </si>
-  <si>
-    <t>Infiltrator</t>
-  </si>
-  <si>
-    <t>When you hire this card, kill one Unit on your opponent's side of the field, then switch control of this card.</t>
-  </si>
-  <si>
-    <t>Treachary</t>
-  </si>
-  <si>
-    <t>Deal 2 damage to all Minions your opponent controls.</t>
-  </si>
-  <si>
-    <t>Hire one Unit from your opponent's side of the field.</t>
-  </si>
-  <si>
-    <t>Shuffle one card back into your deck from your hand, then draw 2 cards.</t>
-  </si>
-  <si>
-    <t>Illusion frog</t>
-  </si>
-  <si>
-    <t>Gain 5 gold.</t>
-  </si>
-  <si>
-    <t>Eldritch Horror</t>
-  </si>
-  <si>
-    <t>Rain of Fire</t>
-  </si>
-  <si>
-    <t>Desperate Times</t>
-  </si>
-  <si>
-    <t>While this unit is on the field, you do not pay wages for your units.</t>
-  </si>
-  <si>
-    <t>Trinkets &amp; Baubles</t>
-  </si>
-  <si>
-    <t>Once per turn, you can pay 1 gold, restore 2 health to a unit on the field.</t>
-  </si>
-  <si>
-    <t>Frog Elder</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">You can pay 3 coins, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>bounce</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> this unit, then search 1 "Frog" card.</t>
     </r>
   </si>
 </sst>
@@ -875,7 +875,7 @@
   <dimension ref="D2:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1091,7 +1091,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K9" t="s">
         <v>39</v>
@@ -1154,7 +1154,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>12</v>
@@ -1169,7 +1169,7 @@
         <v>2</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K12" t="s">
         <v>38</v>
@@ -1180,7 +1180,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>11</v>
@@ -1195,7 +1195,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K13" t="s">
         <v>38</v>
@@ -1258,7 +1258,7 @@
         <v>14</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>12</v>
@@ -1284,7 +1284,7 @@
         <v>15</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>11</v>
@@ -1388,7 +1388,7 @@
         <v>19</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>12</v>
@@ -1403,7 +1403,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="K21" t="s">
         <v>38</v>
@@ -1481,7 +1481,7 @@
         <v>2</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K24" t="s">
         <v>38</v>
@@ -1559,7 +1559,7 @@
         <v>1</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K27" t="s">
         <v>38</v>
@@ -1585,7 +1585,7 @@
         <v>2</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K28" t="s">
         <v>39</v>
@@ -1648,7 +1648,7 @@
         <v>29</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>11</v>
@@ -1663,7 +1663,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K31" t="s">
         <v>38</v>
@@ -1674,7 +1674,7 @@
         <v>30</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>12</v>
@@ -1689,7 +1689,7 @@
         <v>1</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K32" t="s">
         <v>39</v>
@@ -1700,7 +1700,7 @@
         <v>31</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>11</v>
@@ -1715,7 +1715,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K33" t="s">
         <v>39</v>
@@ -1726,7 +1726,7 @@
         <v>32</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>11</v>
@@ -1741,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K34" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Added the Rain Of Fire card
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -312,6 +312,30 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">You can pay 3 coins, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">bounce </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>this unit, then you can take control of 1 minion your opponent controls.</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">You can </t>
     </r>
     <r>
@@ -331,8 +355,56 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>this unit, then deal 2 damage to each of your opponents minions.</t>
-    </r>
+      <t>this unit, place 3 poison counters on an enemy unit.</t>
+    </r>
+  </si>
+  <si>
+    <t>Send a buried minion to it's owner's Discard Pile.</t>
+  </si>
+  <si>
+    <t>Sleight of Hand</t>
+  </si>
+  <si>
+    <t>Infiltrator</t>
+  </si>
+  <si>
+    <t>When you hire this card, kill one Unit on your opponent's side of the field, then switch control of this card.</t>
+  </si>
+  <si>
+    <t>Treachary</t>
+  </si>
+  <si>
+    <t>Hire one Unit from your opponent's side of the field.</t>
+  </si>
+  <si>
+    <t>Shuffle one card back into your deck from your hand, then draw 2 cards.</t>
+  </si>
+  <si>
+    <t>Illusion frog</t>
+  </si>
+  <si>
+    <t>Gain 5 gold.</t>
+  </si>
+  <si>
+    <t>Eldritch Horror</t>
+  </si>
+  <si>
+    <t>Rain of Fire</t>
+  </si>
+  <si>
+    <t>Desperate Times</t>
+  </si>
+  <si>
+    <t>While this unit is on the field, you do not pay wages for your units.</t>
+  </si>
+  <si>
+    <t>Trinkets &amp; Baubles</t>
+  </si>
+  <si>
+    <t>Once per turn, you can pay 1 gold, restore 2 health to a unit on the field.</t>
+  </si>
+  <si>
+    <t>Frog Elder</t>
   </si>
   <si>
     <r>
@@ -346,6 +418,30 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>bounce</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> this unit, then search 1 "Frog" card.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When this minion reaches 0 health from combat, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">bounce </t>
     </r>
     <r>
@@ -355,7 +451,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>this unit, then you can take control of 1 minion your opponent controls.</t>
+      <t>this unit instead of killing it.</t>
     </r>
   </si>
   <si>
@@ -379,107 +475,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>this unit, place 3 poison counters on an enemy unit.</t>
-    </r>
-  </si>
-  <si>
-    <t>Send a buried minion to it's owner's Discard Pile.</t>
-  </si>
-  <si>
-    <t>Sleight of Hand</t>
-  </si>
-  <si>
-    <t>Infiltrator</t>
-  </si>
-  <si>
-    <t>When you hire this card, kill one Unit on your opponent's side of the field, then switch control of this card.</t>
-  </si>
-  <si>
-    <t>Treachary</t>
-  </si>
-  <si>
-    <t>Deal 2 damage to all Minions your opponent controls.</t>
-  </si>
-  <si>
-    <t>Hire one Unit from your opponent's side of the field.</t>
-  </si>
-  <si>
-    <t>Shuffle one card back into your deck from your hand, then draw 2 cards.</t>
-  </si>
-  <si>
-    <t>Illusion frog</t>
-  </si>
-  <si>
-    <t>Gain 5 gold.</t>
-  </si>
-  <si>
-    <t>Eldritch Horror</t>
-  </si>
-  <si>
-    <t>Rain of Fire</t>
-  </si>
-  <si>
-    <t>Desperate Times</t>
-  </si>
-  <si>
-    <t>While this unit is on the field, you do not pay wages for your units.</t>
-  </si>
-  <si>
-    <t>Trinkets &amp; Baubles</t>
-  </si>
-  <si>
-    <t>Once per turn, you can pay 1 gold, restore 2 health to a unit on the field.</t>
-  </si>
-  <si>
-    <t>Frog Elder</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">You can pay 3 coins, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>bounce</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> this unit, then search 1 "Frog" card.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">When this minion reaches 0 health from combat, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">bounce </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>this unit instead of killing it.</t>
-    </r>
+      <t>this unit, then deal 1 damage to each of your opponents minions.</t>
+    </r>
+  </si>
+  <si>
+    <t>Deal 2 damage to all units your opponent controls.</t>
   </si>
 </sst>
 </file>
@@ -875,7 +875,7 @@
   <dimension ref="D2:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1091,7 +1091,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K9" t="s">
         <v>39</v>
@@ -1117,7 +1117,7 @@
         <v>5</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="K10" t="s">
         <v>39</v>
@@ -1143,7 +1143,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K11" t="s">
         <v>39</v>
@@ -1154,7 +1154,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>12</v>
@@ -1169,7 +1169,7 @@
         <v>2</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K12" t="s">
         <v>38</v>
@@ -1180,7 +1180,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>11</v>
@@ -1195,7 +1195,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K13" t="s">
         <v>38</v>
@@ -1258,7 +1258,7 @@
         <v>14</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>12</v>
@@ -1284,7 +1284,7 @@
         <v>15</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>11</v>
@@ -1388,7 +1388,7 @@
         <v>19</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>12</v>
@@ -1403,7 +1403,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K21" t="s">
         <v>38</v>
@@ -1481,7 +1481,7 @@
         <v>2</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K24" t="s">
         <v>38</v>
@@ -1559,7 +1559,7 @@
         <v>1</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K27" t="s">
         <v>38</v>
@@ -1585,7 +1585,7 @@
         <v>2</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K28" t="s">
         <v>39</v>
@@ -1648,7 +1648,7 @@
         <v>29</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>11</v>
@@ -1663,7 +1663,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K31" t="s">
         <v>38</v>
@@ -1674,7 +1674,7 @@
         <v>30</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>12</v>
@@ -1689,7 +1689,7 @@
         <v>1</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K32" t="s">
         <v>39</v>
@@ -1700,7 +1700,7 @@
         <v>31</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>11</v>
@@ -1715,7 +1715,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="K33" t="s">
         <v>39</v>
@@ -1726,7 +1726,7 @@
         <v>32</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>11</v>
@@ -1741,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K34" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Units can now pillage
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -875,7 +875,7 @@
   <dimension ref="D2:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1120,7 +1120,7 @@
         <v>75</v>
       </c>
       <c r="K10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="4:11">
@@ -1718,7 +1718,7 @@
         <v>76</v>
       </c>
       <c r="K33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="4:11">

</xml_diff>

<commit_message>
Implemented the Swelling Flesh card
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -10,11 +10,12 @@
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="79">
   <si>
     <t>Card ID</t>
   </si>
@@ -480,6 +481,12 @@
   </si>
   <si>
     <t>Deal 2 damage to all units your opponent controls.</t>
+  </si>
+  <si>
+    <t>At the end of your turn, increase this unit's strength by 1, and restore 1 health.</t>
+  </si>
+  <si>
+    <t>Swelling Flesh</t>
   </si>
 </sst>
 </file>
@@ -874,14 +881,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D2:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="9.140625" style="7"/>
-    <col min="5" max="5" width="19.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
@@ -1750,6 +1757,24 @@
     <row r="35" spans="4:11">
       <c r="D35" s="7">
         <v>33</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="4">
+        <v>6</v>
+      </c>
+      <c r="H35" s="4">
+        <v>5</v>
+      </c>
+      <c r="I35" s="4">
+        <v>2</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="4:11">

</xml_diff>

<commit_message>
Implemented the Engorgement card
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -10,12 +10,11 @@
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="83">
   <si>
     <t>Card ID</t>
   </si>
@@ -487,6 +486,18 @@
   </si>
   <si>
     <t>Swelling Flesh</t>
+  </si>
+  <si>
+    <t>Swarm of Rats</t>
+  </si>
+  <si>
+    <t>When you summon this unit, search for a copy of "Swarm of Rats".</t>
+  </si>
+  <si>
+    <t>Engorgement</t>
+  </si>
+  <si>
+    <t>Increase the strength of 1 unit on the field by 2.</t>
   </si>
 </sst>
 </file>
@@ -881,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D2:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1776,15 +1787,60 @@
       <c r="J35" s="5" t="s">
         <v>77</v>
       </c>
+      <c r="K35" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="36" spans="4:11">
       <c r="D36" s="7">
         <v>34</v>
       </c>
+      <c r="E36" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="4">
+        <v>3</v>
+      </c>
+      <c r="H36" s="4">
+        <v>2</v>
+      </c>
+      <c r="I36" s="4">
+        <v>2</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="K36" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="37" spans="4:11">
       <c r="D37" s="7">
         <v>35</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="4">
+        <v>3</v>
+      </c>
+      <c r="H37" s="4">
+        <v>0</v>
+      </c>
+      <c r="I37" s="4">
+        <v>0</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K37" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="4:11">

</xml_diff>

<commit_message>
Implemented Swarm of Rats
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -491,13 +491,13 @@
     <t>Swarm of Rats</t>
   </si>
   <si>
-    <t>When you summon this unit, search for a copy of "Swarm of Rats".</t>
-  </si>
-  <si>
     <t>Engorgement</t>
   </si>
   <si>
     <t>Increase the strength of 1 unit on the field by 2.</t>
+  </si>
+  <si>
+    <t>When you summon this unit, search "Swarm of Rats".</t>
   </si>
 </sst>
 </file>
@@ -893,7 +893,7 @@
   <dimension ref="D2:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1811,10 +1811,10 @@
         <v>2</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="K36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="4:11">
@@ -1822,7 +1822,7 @@
         <v>35</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>11</v>
@@ -1837,7 +1837,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K37" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Implemented trigger on event abilities and the Frog Lord card
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -165,7 +165,7 @@
   </si>
   <si>
     <r>
-      <t>Whenever a minion</t>
+      <t>At the end of your turn, you can</t>
     </r>
     <r>
       <rPr>
@@ -175,6 +175,318 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve"> bounce</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> up to 2 minions on your side of the field to your hand.</t>
+    </r>
+  </si>
+  <si>
+    <t>Seismic Frog</t>
+  </si>
+  <si>
+    <t>Sticky Tongue Frog</t>
+  </si>
+  <si>
+    <t>If this card defeats an opponents minion in battle, you can pay 1 coin bury it to your side of the battlefield.</t>
+  </si>
+  <si>
+    <t>Lucky Dip</t>
+  </si>
+  <si>
+    <t>Roll a dice - if the result is a 4, 5 or 6, draw 2 cards.</t>
+  </si>
+  <si>
+    <t>Occult Devotee</t>
+  </si>
+  <si>
+    <t>If you control 5 occult devotees, call upon an "Eldrich Horror" from your hand, deck, or discard pile.</t>
+  </si>
+  <si>
+    <t>Return a Utility in your discard pile to your hand</t>
+  </si>
+  <si>
+    <t>Dying Nobleman</t>
+  </si>
+  <si>
+    <t>Burly Zombie</t>
+  </si>
+  <si>
+    <t>When this minion is called upon, kill all minions on your opponents field, and discard all cards in their hand. This card cannot be summoned by card abilities, except "Occult Devotee".</t>
+  </si>
+  <si>
+    <t>When this minion is killed, gain 6 gold.</t>
+  </si>
+  <si>
+    <t>When this minion is summoned, you can pay 2 gold, ressurect a creature from your discard pile to the battlefield, but put it to 1 health.</t>
+  </si>
+  <si>
+    <t>Black Market</t>
+  </si>
+  <si>
+    <t>Discard a card in your hand and gain gold equal to its cost.</t>
+  </si>
+  <si>
+    <t>Done?</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Mad Scientist</t>
+  </si>
+  <si>
+    <t>Pustulent Zombie</t>
+  </si>
+  <si>
+    <t>When this minion is killed, you can bury it instead. If this minion battles an opponents minion, give it 1 poison counter.</t>
+  </si>
+  <si>
+    <t>Combat Medic</t>
+  </si>
+  <si>
+    <t>Immunity</t>
+  </si>
+  <si>
+    <t>Remove all poison counters from all minions on your side of the field.</t>
+  </si>
+  <si>
+    <t>Antidote</t>
+  </si>
+  <si>
+    <t>Remove all poison counters from a minion on your side of the field.</t>
+  </si>
+  <si>
+    <t>Negotiator</t>
+  </si>
+  <si>
+    <t>Toxic Frog</t>
+  </si>
+  <si>
+    <t>Betrayal</t>
+  </si>
+  <si>
+    <t>Kill a Unit you control, then summon a Unit from your deck with the same cost.</t>
+  </si>
+  <si>
+    <t>When this minion is killed, you can bury it instead. When this minion is ressurected, its strength and health becomes 7.</t>
+  </si>
+  <si>
+    <t>Bloated Body</t>
+  </si>
+  <si>
+    <t>When this unit is killed, deal 3 damage to all other units on the battlefield.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">You can pay 3 coins, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">bounce </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>this unit, then you can take control of 1 minion your opponent controls.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">You can </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">bounce </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>this unit, place 3 poison counters on an enemy unit.</t>
+    </r>
+  </si>
+  <si>
+    <t>Send a buried minion to it's owner's Discard Pile.</t>
+  </si>
+  <si>
+    <t>Sleight of Hand</t>
+  </si>
+  <si>
+    <t>Infiltrator</t>
+  </si>
+  <si>
+    <t>When you hire this card, kill one Unit on your opponent's side of the field, then switch control of this card.</t>
+  </si>
+  <si>
+    <t>Treachary</t>
+  </si>
+  <si>
+    <t>Hire one Unit from your opponent's side of the field.</t>
+  </si>
+  <si>
+    <t>Shuffle one card back into your deck from your hand, then draw 2 cards.</t>
+  </si>
+  <si>
+    <t>Illusion frog</t>
+  </si>
+  <si>
+    <t>Gain 5 gold.</t>
+  </si>
+  <si>
+    <t>Eldritch Horror</t>
+  </si>
+  <si>
+    <t>Rain of Fire</t>
+  </si>
+  <si>
+    <t>Desperate Times</t>
+  </si>
+  <si>
+    <t>While this unit is on the field, you do not pay wages for your units.</t>
+  </si>
+  <si>
+    <t>Trinkets &amp; Baubles</t>
+  </si>
+  <si>
+    <t>Once per turn, you can pay 1 gold, restore 2 health to a unit on the field.</t>
+  </si>
+  <si>
+    <t>Frog Elder</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">You can pay 3 coins, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bounce</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> this unit, then search 1 "Frog" card.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When this minion reaches 0 health from combat, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">bounce </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>this unit instead of killing it.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">You can </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">bounce </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>this unit, then deal 1 damage to each of your opponents minions.</t>
+    </r>
+  </si>
+  <si>
+    <t>Deal 2 damage to all units your opponent controls.</t>
+  </si>
+  <si>
+    <t>At the end of your turn, increase this unit's strength by 1, and restore 1 health.</t>
+  </si>
+  <si>
+    <t>Swelling Flesh</t>
+  </si>
+  <si>
+    <t>Swarm of Rats</t>
+  </si>
+  <si>
+    <t>Engorgement</t>
+  </si>
+  <si>
+    <t>Increase the strength of 1 unit on the field by 2.</t>
+  </si>
+  <si>
+    <t>When you summon this unit, search "Swarm of Rats".</t>
+  </si>
+  <si>
+    <r>
+      <t>Once per turn when a unit</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> bounces</t>
     </r>
     <r>
@@ -184,320 +496,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> to your hand from your side of the field, draw 1 card.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>At the end of your turn, you can</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> bounce</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> up to 2 minions on your side of the field to your hand.</t>
-    </r>
-  </si>
-  <si>
-    <t>Seismic Frog</t>
-  </si>
-  <si>
-    <t>Sticky Tongue Frog</t>
-  </si>
-  <si>
-    <t>If this card defeats an opponents minion in battle, you can pay 1 coin bury it to your side of the battlefield.</t>
-  </si>
-  <si>
-    <t>Lucky Dip</t>
-  </si>
-  <si>
-    <t>Roll a dice - if the result is a 4, 5 or 6, draw 2 cards.</t>
-  </si>
-  <si>
-    <t>Occult Devotee</t>
-  </si>
-  <si>
-    <t>If you control 5 occult devotees, call upon an "Eldrich Horror" from your hand, deck, or discard pile.</t>
-  </si>
-  <si>
-    <t>Return a Utility in your discard pile to your hand</t>
-  </si>
-  <si>
-    <t>Dying Nobleman</t>
-  </si>
-  <si>
-    <t>Burly Zombie</t>
-  </si>
-  <si>
-    <t>When this minion is called upon, kill all minions on your opponents field, and discard all cards in their hand. This card cannot be summoned by card abilities, except "Occult Devotee".</t>
-  </si>
-  <si>
-    <t>When this minion is killed, gain 6 gold.</t>
-  </si>
-  <si>
-    <t>When this minion is summoned, you can pay 2 gold, ressurect a creature from your discard pile to the battlefield, but put it to 1 health.</t>
-  </si>
-  <si>
-    <t>Black Market</t>
-  </si>
-  <si>
-    <t>Discard a card in your hand and gain gold equal to its cost.</t>
-  </si>
-  <si>
-    <t>Done?</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Mad Scientist</t>
-  </si>
-  <si>
-    <t>Pustulent Zombie</t>
-  </si>
-  <si>
-    <t>When this minion is killed, you can bury it instead. If this minion battles an opponents minion, give it 1 poison counter.</t>
-  </si>
-  <si>
-    <t>Combat Medic</t>
-  </si>
-  <si>
-    <t>Immunity</t>
-  </si>
-  <si>
-    <t>Remove all poison counters from all minions on your side of the field.</t>
-  </si>
-  <si>
-    <t>Antidote</t>
-  </si>
-  <si>
-    <t>Remove all poison counters from a minion on your side of the field.</t>
-  </si>
-  <si>
-    <t>Negotiator</t>
-  </si>
-  <si>
-    <t>Toxic Frog</t>
-  </si>
-  <si>
-    <t>Betrayal</t>
-  </si>
-  <si>
-    <t>Kill a Unit you control, then summon a Unit from your deck with the same cost.</t>
-  </si>
-  <si>
-    <t>When this minion is killed, you can bury it instead. When this minion is ressurected, its strength and health becomes 7.</t>
-  </si>
-  <si>
-    <t>Bloated Body</t>
-  </si>
-  <si>
-    <t>When this unit is killed, deal 3 damage to all other units on the battlefield.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">You can pay 3 coins, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">bounce </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>this unit, then you can take control of 1 minion your opponent controls.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">You can </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">bounce </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>this unit, place 3 poison counters on an enemy unit.</t>
-    </r>
-  </si>
-  <si>
-    <t>Send a buried minion to it's owner's Discard Pile.</t>
-  </si>
-  <si>
-    <t>Sleight of Hand</t>
-  </si>
-  <si>
-    <t>Infiltrator</t>
-  </si>
-  <si>
-    <t>When you hire this card, kill one Unit on your opponent's side of the field, then switch control of this card.</t>
-  </si>
-  <si>
-    <t>Treachary</t>
-  </si>
-  <si>
-    <t>Hire one Unit from your opponent's side of the field.</t>
-  </si>
-  <si>
-    <t>Shuffle one card back into your deck from your hand, then draw 2 cards.</t>
-  </si>
-  <si>
-    <t>Illusion frog</t>
-  </si>
-  <si>
-    <t>Gain 5 gold.</t>
-  </si>
-  <si>
-    <t>Eldritch Horror</t>
-  </si>
-  <si>
-    <t>Rain of Fire</t>
-  </si>
-  <si>
-    <t>Desperate Times</t>
-  </si>
-  <si>
-    <t>While this unit is on the field, you do not pay wages for your units.</t>
-  </si>
-  <si>
-    <t>Trinkets &amp; Baubles</t>
-  </si>
-  <si>
-    <t>Once per turn, you can pay 1 gold, restore 2 health to a unit on the field.</t>
-  </si>
-  <si>
-    <t>Frog Elder</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">You can pay 3 coins, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>bounce</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> this unit, then search 1 "Frog" card.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">When this minion reaches 0 health from combat, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">bounce </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>this unit instead of killing it.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">You can </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">bounce </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>this unit, then deal 1 damage to each of your opponents minions.</t>
-    </r>
-  </si>
-  <si>
-    <t>Deal 2 damage to all units your opponent controls.</t>
-  </si>
-  <si>
-    <t>At the end of your turn, increase this unit's strength by 1, and restore 1 health.</t>
-  </si>
-  <si>
-    <t>Swelling Flesh</t>
-  </si>
-  <si>
-    <t>Swarm of Rats</t>
-  </si>
-  <si>
-    <t>Engorgement</t>
-  </si>
-  <si>
-    <t>Increase the strength of 1 unit on the field by 2.</t>
-  </si>
-  <si>
-    <t>When you summon this unit, search "Swarm of Rats".</t>
+      <t xml:space="preserve"> to your hand, draw 1 card.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -892,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D2:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -930,7 +930,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="4:11">
@@ -953,10 +953,10 @@
         <v>0</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="4:11">
@@ -979,10 +979,10 @@
         <v>0</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="K4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="4:11">
@@ -1008,7 +1008,7 @@
         <v>19</v>
       </c>
       <c r="K5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="4:11">
@@ -1034,7 +1034,7 @@
         <v>18</v>
       </c>
       <c r="K6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="4:11">
@@ -1060,7 +1060,7 @@
         <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="4:11">
@@ -1083,10 +1083,10 @@
         <v>2</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="4:11">
@@ -1109,10 +1109,10 @@
         <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="4:11">
@@ -1120,7 +1120,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>12</v>
@@ -1135,10 +1135,10 @@
         <v>5</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="4:11">
@@ -1146,7 +1146,7 @@
         <v>9</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>12</v>
@@ -1161,10 +1161,10 @@
         <v>1</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="4:11">
@@ -1172,7 +1172,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>12</v>
@@ -1187,10 +1187,10 @@
         <v>2</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="4:11">
@@ -1198,7 +1198,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>11</v>
@@ -1213,10 +1213,10 @@
         <v>0</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="4:11">
@@ -1224,7 +1224,7 @@
         <v>12</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>11</v>
@@ -1239,10 +1239,10 @@
         <v>0</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="4:11">
@@ -1250,7 +1250,7 @@
         <v>13</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>12</v>
@@ -1265,10 +1265,10 @@
         <v>2</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="4:11">
@@ -1276,7 +1276,7 @@
         <v>14</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>12</v>
@@ -1291,10 +1291,10 @@
         <v>30</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="4:11">
@@ -1302,7 +1302,7 @@
         <v>15</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>11</v>
@@ -1317,10 +1317,10 @@
         <v>0</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="4:11">
@@ -1328,7 +1328,7 @@
         <v>16</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>12</v>
@@ -1343,10 +1343,10 @@
         <v>1</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="4:11">
@@ -1354,7 +1354,7 @@
         <v>17</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>12</v>
@@ -1369,10 +1369,10 @@
         <v>3</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="4:11">
@@ -1380,7 +1380,7 @@
         <v>18</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>12</v>
@@ -1395,10 +1395,10 @@
         <v>5</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="4:11">
@@ -1406,7 +1406,7 @@
         <v>19</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>12</v>
@@ -1421,10 +1421,10 @@
         <v>2</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="4:11">
@@ -1432,7 +1432,7 @@
         <v>20</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>11</v>
@@ -1447,10 +1447,10 @@
         <v>0</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="4:11">
@@ -1458,7 +1458,7 @@
         <v>21</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>12</v>
@@ -1473,10 +1473,10 @@
         <v>1</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="4:11">
@@ -1484,7 +1484,7 @@
         <v>22</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>12</v>
@@ -1499,10 +1499,10 @@
         <v>2</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="4:11">
@@ -1510,7 +1510,7 @@
         <v>23</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>11</v>
@@ -1525,10 +1525,10 @@
         <v>0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="4:11">
@@ -1536,7 +1536,7 @@
         <v>24</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>11</v>
@@ -1551,10 +1551,10 @@
         <v>0</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="4:11">
@@ -1562,7 +1562,7 @@
         <v>25</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>12</v>
@@ -1577,10 +1577,10 @@
         <v>1</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="4:11">
@@ -1588,7 +1588,7 @@
         <v>26</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>12</v>
@@ -1603,10 +1603,10 @@
         <v>2</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="4:11">
@@ -1614,7 +1614,7 @@
         <v>27</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>11</v>
@@ -1629,10 +1629,10 @@
         <v>0</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="4:11">
@@ -1640,7 +1640,7 @@
         <v>28</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>12</v>
@@ -1655,10 +1655,10 @@
         <v>1</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="4:11">
@@ -1666,7 +1666,7 @@
         <v>29</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>11</v>
@@ -1681,10 +1681,10 @@
         <v>0</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="4:11">
@@ -1692,7 +1692,7 @@
         <v>30</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>12</v>
@@ -1707,10 +1707,10 @@
         <v>1</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="4:11">
@@ -1718,7 +1718,7 @@
         <v>31</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>11</v>
@@ -1733,10 +1733,10 @@
         <v>0</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="4:11">
@@ -1744,7 +1744,7 @@
         <v>32</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>11</v>
@@ -1759,10 +1759,10 @@
         <v>0</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="4:11">
@@ -1770,7 +1770,7 @@
         <v>33</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>12</v>
@@ -1785,10 +1785,10 @@
         <v>2</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="4:11">
@@ -1796,7 +1796,7 @@
         <v>34</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>12</v>
@@ -1811,10 +1811,10 @@
         <v>2</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="4:11">
@@ -1822,7 +1822,7 @@
         <v>35</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>11</v>
@@ -1837,10 +1837,10 @@
         <v>0</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="4:11">

</xml_diff>

<commit_message>
Implemented the Medicine card
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="87">
   <si>
     <t>Card ID</t>
   </si>
@@ -498,6 +498,18 @@
       </rPr>
       <t xml:space="preserve"> to your hand, draw 1 card.</t>
     </r>
+  </si>
+  <si>
+    <t>The Healer</t>
+  </si>
+  <si>
+    <t>At the end of your turn, heal 1 unit you control to full health.</t>
+  </si>
+  <si>
+    <t>Fully restore 1 unit's health.</t>
+  </si>
+  <si>
+    <t>Medicine</t>
   </si>
 </sst>
 </file>
@@ -892,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D2:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1847,9 +1859,51 @@
       <c r="D38" s="7">
         <v>36</v>
       </c>
+      <c r="E38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" s="4">
+        <v>0</v>
+      </c>
+      <c r="H38" s="4">
+        <v>0</v>
+      </c>
+      <c r="I38" s="4">
+        <v>0</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K38" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="39" spans="4:11">
       <c r="D39" s="7">
+        <v>37</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="4">
+        <v>3</v>
+      </c>
+      <c r="H39" s="4">
+        <v>0</v>
+      </c>
+      <c r="I39" s="4">
+        <v>0</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="K39" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented the Assassination card
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="89">
   <si>
     <t>Card ID</t>
   </si>
@@ -203,12 +203,6 @@
     <t>Roll a dice - if the result is a 4, 5 or 6, draw 2 cards.</t>
   </si>
   <si>
-    <t>Occult Devotee</t>
-  </si>
-  <si>
-    <t>If you control 5 occult devotees, call upon an "Eldrich Horror" from your hand, deck, or discard pile.</t>
-  </si>
-  <si>
     <t>Return a Utility in your discard pile to your hand</t>
   </si>
   <si>
@@ -216,9 +210,6 @@
   </si>
   <si>
     <t>Burly Zombie</t>
-  </si>
-  <si>
-    <t>When this minion is called upon, kill all minions on your opponents field, and discard all cards in their hand. This card cannot be summoned by card abilities, except "Occult Devotee".</t>
   </si>
   <si>
     <t>When this minion is killed, gain 6 gold.</t>
@@ -500,9 +491,6 @@
     </r>
   </si>
   <si>
-    <t>The Healer</t>
-  </si>
-  <si>
     <t>At the end of your turn, heal 1 unit you control to full health.</t>
   </si>
   <si>
@@ -510,6 +498,24 @@
   </si>
   <si>
     <t>Medicine</t>
+  </si>
+  <si>
+    <t>If you control 3 occult devotees at the end of your turn, summon this card with 30 health and 30 strength.</t>
+  </si>
+  <si>
+    <t>Eldritch Devotee</t>
+  </si>
+  <si>
+    <t>At the end of your turn, search 1 "Devoted Cultist"</t>
+  </si>
+  <si>
+    <t>Assasination</t>
+  </si>
+  <si>
+    <t>Kill an undamaged unit.</t>
+  </si>
+  <si>
+    <t>The Doctor</t>
   </si>
 </sst>
 </file>
@@ -904,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D2:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -942,7 +948,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="4:11">
@@ -968,7 +974,7 @@
         <v>20</v>
       </c>
       <c r="K3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="4:11">
@@ -991,10 +997,10 @@
         <v>0</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="4:11">
@@ -1020,7 +1026,7 @@
         <v>19</v>
       </c>
       <c r="K5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="4:11">
@@ -1046,7 +1052,7 @@
         <v>18</v>
       </c>
       <c r="K6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="4:11">
@@ -1072,7 +1078,7 @@
         <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="4:11">
@@ -1098,7 +1104,7 @@
         <v>23</v>
       </c>
       <c r="K8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="4:11">
@@ -1121,10 +1127,10 @@
         <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="4:11">
@@ -1147,10 +1153,10 @@
         <v>5</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="K10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="4:11">
@@ -1173,10 +1179,10 @@
         <v>1</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="4:11">
@@ -1184,7 +1190,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>12</v>
@@ -1199,10 +1205,10 @@
         <v>2</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="4:11">
@@ -1210,7 +1216,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>11</v>
@@ -1225,10 +1231,10 @@
         <v>0</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="4:11">
@@ -1254,15 +1260,15 @@
         <v>25</v>
       </c>
       <c r="K14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="4:11">
       <c r="D15" s="7">
         <v>13</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>26</v>
+      <c r="E15" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>12</v>
@@ -1277,10 +1283,10 @@
         <v>2</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="K15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="4:11">
@@ -1288,13 +1294,13 @@
         <v>14</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G16" s="4">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="H16" s="4">
         <v>30</v>
@@ -1303,10 +1309,10 @@
         <v>30</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="K16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="4:11">
@@ -1314,7 +1320,7 @@
         <v>15</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>11</v>
@@ -1329,10 +1335,10 @@
         <v>0</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="4:11">
@@ -1340,7 +1346,7 @@
         <v>16</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>12</v>
@@ -1355,10 +1361,10 @@
         <v>1</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="4:11">
@@ -1366,7 +1372,7 @@
         <v>17</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>12</v>
@@ -1381,10 +1387,10 @@
         <v>3</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="4:11">
@@ -1392,7 +1398,7 @@
         <v>18</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>12</v>
@@ -1407,10 +1413,10 @@
         <v>5</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="K20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="4:11">
@@ -1418,7 +1424,7 @@
         <v>19</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>12</v>
@@ -1433,10 +1439,10 @@
         <v>2</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="4:11">
@@ -1444,7 +1450,7 @@
         <v>20</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>11</v>
@@ -1459,10 +1465,10 @@
         <v>0</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="4:11">
@@ -1470,7 +1476,7 @@
         <v>21</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>12</v>
@@ -1485,10 +1491,10 @@
         <v>1</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="4:11">
@@ -1496,7 +1502,7 @@
         <v>22</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>12</v>
@@ -1511,10 +1517,10 @@
         <v>2</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K24" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="4:11">
@@ -1522,7 +1528,7 @@
         <v>23</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>11</v>
@@ -1537,10 +1543,10 @@
         <v>0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K25" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="4:11">
@@ -1548,7 +1554,7 @@
         <v>24</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>11</v>
@@ -1563,10 +1569,10 @@
         <v>0</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K26" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="4:11">
@@ -1574,7 +1580,7 @@
         <v>25</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>12</v>
@@ -1589,10 +1595,10 @@
         <v>1</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K27" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="4:11">
@@ -1600,7 +1606,7 @@
         <v>26</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>12</v>
@@ -1615,10 +1621,10 @@
         <v>2</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K28" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="4:11">
@@ -1626,7 +1632,7 @@
         <v>27</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>11</v>
@@ -1641,10 +1647,10 @@
         <v>0</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K29" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="4:11">
@@ -1652,7 +1658,7 @@
         <v>28</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>12</v>
@@ -1667,10 +1673,10 @@
         <v>1</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="4:11">
@@ -1678,7 +1684,7 @@
         <v>29</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>11</v>
@@ -1693,10 +1699,10 @@
         <v>0</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K31" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="4:11">
@@ -1704,7 +1710,7 @@
         <v>30</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>12</v>
@@ -1719,10 +1725,10 @@
         <v>1</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K32" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="4:11">
@@ -1730,7 +1736,7 @@
         <v>31</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>11</v>
@@ -1745,10 +1751,10 @@
         <v>0</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="K33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="4:11">
@@ -1756,7 +1762,7 @@
         <v>32</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>11</v>
@@ -1771,10 +1777,10 @@
         <v>0</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="4:11">
@@ -1782,7 +1788,7 @@
         <v>33</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>12</v>
@@ -1797,10 +1803,10 @@
         <v>2</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K35" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="4:11">
@@ -1808,7 +1814,7 @@
         <v>34</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>12</v>
@@ -1823,10 +1829,10 @@
         <v>2</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K36" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="4:11">
@@ -1834,7 +1840,7 @@
         <v>35</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>11</v>
@@ -1849,10 +1855,10 @@
         <v>0</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K37" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="4:11">
@@ -1860,7 +1866,7 @@
         <v>36</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>5</v>
@@ -1875,10 +1881,10 @@
         <v>0</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="K38" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="4:11">
@@ -1886,7 +1892,7 @@
         <v>37</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>11</v>
@@ -1901,15 +1907,36 @@
         <v>0</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="K39" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="4:11">
       <c r="D40" s="7">
         <v>38</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="4">
+        <v>5</v>
+      </c>
+      <c r="H40" s="4">
+        <v>0</v>
+      </c>
+      <c r="I40" s="4">
+        <v>0</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K40" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="4:11">

</xml_diff>

<commit_message>
Implemented the Assassin card
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="93">
   <si>
     <t>Card ID</t>
   </si>
@@ -491,9 +491,6 @@
     </r>
   </si>
   <si>
-    <t>At the end of your turn, heal 1 unit you control to full health.</t>
-  </si>
-  <si>
     <t>Fully restore 1 unit's health.</t>
   </si>
   <si>
@@ -516,6 +513,21 @@
   </si>
   <si>
     <t>The Doctor</t>
+  </si>
+  <si>
+    <t>Assassin</t>
+  </si>
+  <si>
+    <t>When you summon this unit, search "Assassination"</t>
+  </si>
+  <si>
+    <t>At the end of your turn, restore 1 health to all units on your side of the field.</t>
+  </si>
+  <si>
+    <t>The Contract</t>
+  </si>
+  <si>
+    <t>At the end of your opponent's turns, search "Assassin".</t>
   </si>
 </sst>
 </file>
@@ -910,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D2:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1268,7 +1280,7 @@
         <v>13</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>12</v>
@@ -1283,7 +1295,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K15" t="s">
         <v>35</v>
@@ -1309,7 +1321,7 @@
         <v>30</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K16" t="s">
         <v>35</v>
@@ -1866,7 +1878,7 @@
         <v>36</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>5</v>
@@ -1881,7 +1893,7 @@
         <v>0</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="K38" t="s">
         <v>35</v>
@@ -1892,7 +1904,7 @@
         <v>37</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>11</v>
@@ -1907,7 +1919,7 @@
         <v>0</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K39" t="s">
         <v>34</v>
@@ -1918,7 +1930,7 @@
         <v>38</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>11</v>
@@ -1933,20 +1945,62 @@
         <v>0</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="4:11">
       <c r="D41" s="7">
         <v>39</v>
       </c>
+      <c r="E41" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="4">
+        <v>3</v>
+      </c>
+      <c r="H41" s="4">
+        <v>1</v>
+      </c>
+      <c r="I41" s="4">
+        <v>4</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K41" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="42" spans="4:11">
       <c r="D42" s="7">
         <v>40</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="4">
+        <v>0</v>
+      </c>
+      <c r="H42" s="4">
+        <v>0</v>
+      </c>
+      <c r="I42" s="4">
+        <v>0</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="K42" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="4:11">

</xml_diff>

<commit_message>
Implemented the 'Banishment' card
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="97">
   <si>
     <t>Card ID</t>
   </si>
@@ -528,6 +528,18 @@
   </si>
   <si>
     <t>At the end of your opponent's turns, search "Assassin".</t>
+  </si>
+  <si>
+    <t>Banishment</t>
+  </si>
+  <si>
+    <t>Cannibal</t>
+  </si>
+  <si>
+    <t>Once per turn, you can kill one of your units, fully restore this unit's health.</t>
+  </si>
+  <si>
+    <t>Shuffle one unit on the field into its player's deck.</t>
   </si>
 </sst>
 </file>
@@ -922,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D2:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" topLeftCell="E16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2000,17 +2012,59 @@
         <v>92</v>
       </c>
       <c r="K42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="4:11">
       <c r="D43" s="7">
         <v>41</v>
       </c>
+      <c r="E43" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="4">
+        <v>5</v>
+      </c>
+      <c r="H43" s="4">
+        <v>0</v>
+      </c>
+      <c r="I43" s="4">
+        <v>0</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="K43" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="44" spans="4:11">
       <c r="D44" s="7">
         <v>42</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="4">
+        <v>3</v>
+      </c>
+      <c r="H44" s="4">
+        <v>4</v>
+      </c>
+      <c r="I44" s="4">
+        <v>1</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="K44" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="4:11">

</xml_diff>

<commit_message>
Implemented the 'Cannibal' card
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -536,10 +536,10 @@
     <t>Cannibal</t>
   </si>
   <si>
-    <t>Once per turn, you can kill one of your units, fully restore this unit's health.</t>
-  </si>
-  <si>
     <t>Shuffle one unit on the field into its player's deck.</t>
+  </si>
+  <si>
+    <t>Once per turn, you can kill one of your other units, fully heal this unit.</t>
   </si>
 </sst>
 </file>
@@ -935,7 +935,7 @@
   <dimension ref="D2:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2035,7 +2035,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K43" t="s">
         <v>34</v>
@@ -2061,10 +2061,10 @@
         <v>1</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="4:11">

</xml_diff>

<commit_message>
Added the 'Grave Robber' card to the card spreadsheet
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="99">
   <si>
     <t>Card ID</t>
   </si>
@@ -540,6 +540,12 @@
   </si>
   <si>
     <t>Once per turn, you can kill one of your other units, fully heal this unit.</t>
+  </si>
+  <si>
+    <t>Grave Robber</t>
+  </si>
+  <si>
+    <t>When this unit is killed, steal 2 gold.</t>
   </si>
 </sst>
 </file>
@@ -935,7 +941,7 @@
   <dimension ref="D2:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2070,6 +2076,24 @@
     <row r="45" spans="4:11">
       <c r="D45" s="7">
         <v>43</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" s="4">
+        <v>4</v>
+      </c>
+      <c r="H45" s="4">
+        <v>2</v>
+      </c>
+      <c r="I45" s="4">
+        <v>2</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="4:11">

</xml_diff>

<commit_message>
Added the ability to filter cards by cost in the deckbuilder
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="101">
   <si>
     <t>Card ID</t>
   </si>
@@ -546,6 +546,12 @@
   </si>
   <si>
     <t>When this unit is killed, steal 2 gold.</t>
+  </si>
+  <si>
+    <t>Glancing Blow</t>
+  </si>
+  <si>
+    <t>Deal 2 damage to one unit.</t>
   </si>
 </sst>
 </file>
@@ -941,7 +947,7 @@
   <dimension ref="D2:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2095,10 +2101,34 @@
       <c r="J45" s="5" t="s">
         <v>98</v>
       </c>
+      <c r="K45" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="46" spans="4:11">
       <c r="D46" s="7">
         <v>44</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="4">
+        <v>1</v>
+      </c>
+      <c r="H46" s="4">
+        <v>0</v>
+      </c>
+      <c r="I46" s="4">
+        <v>0</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="K46" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="4:11">

</xml_diff>

<commit_message>
Begun work on the context section of the report, reworded some parts of the Project Management section
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -239,9 +239,6 @@
     <t>Pustulent Zombie</t>
   </si>
   <si>
-    <t>When this minion is killed, you can bury it instead. If this minion battles an opponents minion, give it 1 poison counter.</t>
-  </si>
-  <si>
     <t>Combat Medic</t>
   </si>
   <si>
@@ -503,9 +500,6 @@
     <t>Eldritch Devotee</t>
   </si>
   <si>
-    <t>At the end of your turn, search 1 "Devoted Cultist"</t>
-  </si>
-  <si>
     <t>Assasination</t>
   </si>
   <si>
@@ -557,7 +551,13 @@
     <t>Bloodsucker</t>
   </si>
   <si>
-    <t>When this unit attacks and opponent's unit, fully restore this unit's health.</t>
+    <t>At the end of your turn, search 1 "Eldritch Devotee"</t>
+  </si>
+  <si>
+    <t>After this unit attacks an opponent's unit, fully restore this unit's health.</t>
+  </si>
+  <si>
+    <t>If this minion battles an opponents minion, give it 1 poison counter.</t>
   </si>
 </sst>
 </file>
@@ -952,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D2:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1039,7 +1039,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K4" t="s">
         <v>34</v>
@@ -1169,7 +1169,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K9" t="s">
         <v>35</v>
@@ -1195,7 +1195,7 @@
         <v>5</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K10" t="s">
         <v>34</v>
@@ -1221,7 +1221,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K11" t="s">
         <v>35</v>
@@ -1232,7 +1232,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>12</v>
@@ -1247,7 +1247,7 @@
         <v>2</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K12" t="s">
         <v>34</v>
@@ -1258,7 +1258,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>11</v>
@@ -1273,7 +1273,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K13" t="s">
         <v>34</v>
@@ -1310,7 +1310,7 @@
         <v>13</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>12</v>
@@ -1325,7 +1325,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="K15" t="s">
         <v>35</v>
@@ -1336,7 +1336,7 @@
         <v>14</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>5</v>
@@ -1351,7 +1351,7 @@
         <v>30</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K16" t="s">
         <v>35</v>
@@ -1362,7 +1362,7 @@
         <v>15</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>11</v>
@@ -1455,7 +1455,7 @@
         <v>5</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K20" t="s">
         <v>35</v>
@@ -1466,7 +1466,7 @@
         <v>19</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>12</v>
@@ -1481,7 +1481,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K21" t="s">
         <v>34</v>
@@ -1533,7 +1533,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="K23" t="s">
         <v>35</v>
@@ -1544,7 +1544,7 @@
         <v>22</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>12</v>
@@ -1559,7 +1559,7 @@
         <v>2</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K24" t="s">
         <v>34</v>
@@ -1570,7 +1570,7 @@
         <v>23</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>11</v>
@@ -1585,7 +1585,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K25" t="s">
         <v>35</v>
@@ -1596,7 +1596,7 @@
         <v>24</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>11</v>
@@ -1611,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K26" t="s">
         <v>35</v>
@@ -1622,7 +1622,7 @@
         <v>25</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>12</v>
@@ -1637,7 +1637,7 @@
         <v>1</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K27" t="s">
         <v>34</v>
@@ -1648,7 +1648,7 @@
         <v>26</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>12</v>
@@ -1663,7 +1663,7 @@
         <v>2</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K28" t="s">
         <v>35</v>
@@ -1674,7 +1674,7 @@
         <v>27</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>11</v>
@@ -1689,7 +1689,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K29" t="s">
         <v>35</v>
@@ -1700,7 +1700,7 @@
         <v>28</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>12</v>
@@ -1715,7 +1715,7 @@
         <v>1</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K30" t="s">
         <v>34</v>
@@ -1726,7 +1726,7 @@
         <v>29</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>11</v>
@@ -1741,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K31" t="s">
         <v>34</v>
@@ -1752,7 +1752,7 @@
         <v>30</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>12</v>
@@ -1767,7 +1767,7 @@
         <v>1</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K32" t="s">
         <v>35</v>
@@ -1778,7 +1778,7 @@
         <v>31</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>11</v>
@@ -1793,7 +1793,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K33" t="s">
         <v>34</v>
@@ -1804,7 +1804,7 @@
         <v>32</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>11</v>
@@ -1819,7 +1819,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K34" t="s">
         <v>35</v>
@@ -1830,7 +1830,7 @@
         <v>33</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>12</v>
@@ -1845,7 +1845,7 @@
         <v>2</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K35" t="s">
         <v>34</v>
@@ -1856,7 +1856,7 @@
         <v>34</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>12</v>
@@ -1871,7 +1871,7 @@
         <v>2</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K36" t="s">
         <v>34</v>
@@ -1882,7 +1882,7 @@
         <v>35</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>11</v>
@@ -1897,7 +1897,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K37" t="s">
         <v>34</v>
@@ -1908,7 +1908,7 @@
         <v>36</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>5</v>
@@ -1923,10 +1923,10 @@
         <v>0</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="4:11">
@@ -1934,7 +1934,7 @@
         <v>37</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>11</v>
@@ -1949,7 +1949,7 @@
         <v>0</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K39" t="s">
         <v>34</v>
@@ -1960,7 +1960,7 @@
         <v>38</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>11</v>
@@ -1975,7 +1975,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K40" t="s">
         <v>34</v>
@@ -1986,7 +1986,7 @@
         <v>39</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>12</v>
@@ -2001,7 +2001,7 @@
         <v>4</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K41" t="s">
         <v>34</v>
@@ -2012,7 +2012,7 @@
         <v>40</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>5</v>
@@ -2027,7 +2027,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K42" t="s">
         <v>34</v>
@@ -2038,7 +2038,7 @@
         <v>41</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>11</v>
@@ -2053,7 +2053,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K43" t="s">
         <v>34</v>
@@ -2064,7 +2064,7 @@
         <v>42</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>12</v>
@@ -2079,7 +2079,7 @@
         <v>1</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K44" t="s">
         <v>34</v>
@@ -2090,7 +2090,7 @@
         <v>43</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>12</v>
@@ -2105,7 +2105,7 @@
         <v>2</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K45" t="s">
         <v>34</v>
@@ -2116,7 +2116,7 @@
         <v>44</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>11</v>
@@ -2131,7 +2131,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K46" t="s">
         <v>34</v>
@@ -2142,7 +2142,7 @@
         <v>45</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>12</v>
@@ -2157,10 +2157,10 @@
         <v>3</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="4:11">

</xml_diff>